<commit_message>
working on prompt and excel input
</commit_message>
<xml_diff>
--- a/taks.xlsx
+++ b/taks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaha\Projects\Python Projects\TAKAutomator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B25ED80-A4AC-4F78-9C06-F1536B222B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7DB7DB-D96D-45FC-8AE4-ABDED43DAD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="70">
   <si>
     <t>TYPE</t>
   </si>
@@ -209,12 +209,6 @@
     <t>["Severe hypoglycemia", "Hypoglycemia", "Low glucose", "Normal glucose", "High glucose", "Hyperglycemia"]</t>
   </si>
   <si>
-    <t>GOOD_BEFORE_UNIT</t>
-  </si>
-  <si>
-    <t>GOOD_AFTER_UNIT</t>
-  </si>
-  <si>
     <t>hours</t>
   </si>
   <si>
@@ -266,22 +260,22 @@
     <t>seconds</t>
   </si>
   <si>
-    <t>PERSISTENCE_BEHAVIOR</t>
-  </si>
-  <si>
     <t>pos-pos</t>
-  </si>
-  <si>
-    <t>INTERPOLATION_ROWS</t>
-  </si>
-  <si>
-    <t>GLOBAL_PERSISTENCE</t>
   </si>
   <si>
     <t>OUTPUT_TYPES</t>
   </si>
   <si>
     <t>ordinal</t>
+  </si>
+  <si>
+    <t>GOOD_BEFORE_GRANULARITY</t>
+  </si>
+  <si>
+    <t>GOOD_AFTER_GRANULARITY</t>
+  </si>
+  <si>
+    <t>GLOBAL_BEHAVIOUR</t>
   </si>
 </sst>
 </file>
@@ -671,9 +665,9 @@
   </sheetPr>
   <dimension ref="A1:W908"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -701,13 +695,13 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>28</v>
@@ -728,13 +722,13 @@
         <v>41</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>42</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>15</v>
@@ -755,7 +749,7 @@
         <v>35</v>
       </c>
       <c r="V1" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>36</v>
@@ -769,36 +763,36 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="str" cm="1">
         <f t="array" ref="D2">INDEX(_xlfn.TEXTSPLIT(C2, "-"), 1)</f>
         <v>nominal</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L2" s="3">
         <v>0</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N2" s="3">
         <v>0</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P2" s="2" t="b">
         <v>1</v>
@@ -829,36 +823,36 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3" s="2" t="str" cm="1">
         <f t="array" ref="D3">INDEX(_xlfn.TEXTSPLIT(C3, "-"), 1)</f>
         <v>nominal</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L3" s="3">
         <v>0</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N3" s="3">
         <v>0</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P3" s="2" t="b">
         <v>1</v>
@@ -889,36 +883,36 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="str" cm="1">
         <f t="array" ref="D4">INDEX(_xlfn.TEXTSPLIT(C4, "-"), 1)</f>
         <v>nominal</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L4" s="3">
         <v>0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P4" s="2" t="b">
         <v>1</v>
@@ -949,36 +943,36 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="2" t="str" cm="1">
         <f t="array" ref="D5">INDEX(_xlfn.TEXTSPLIT(C5, "-"), 1)</f>
         <v>nominal</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L5" s="3">
         <v>0</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N5" s="3">
         <v>0</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P5" s="2" t="b">
         <v>1</v>
@@ -1009,17 +1003,17 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6" s="2" t="str" cm="1">
         <f t="array" ref="D6">INDEX(_xlfn.TEXTSPLIT(C6, "-"), 1)</f>
         <v>numeric</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G6" s="2">
         <v>20</v>
@@ -1038,13 +1032,13 @@
         <v>0</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N6" s="3">
         <v>6</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P6" s="2" t="b">
         <v>1</v>
@@ -1075,17 +1069,17 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" s="2" t="str" cm="1">
         <f t="array" ref="D7">INDEX(_xlfn.TEXTSPLIT(C7, "-"), 1)</f>
         <v>numeric</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G7" s="2">
         <v>20</v>
@@ -1104,13 +1098,13 @@
         <v>0</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N7" s="2">
         <v>4</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P7" s="2" t="b">
         <v>1</v>
@@ -1141,36 +1135,36 @@
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" s="2" t="str" cm="1">
         <f t="array" ref="D8">INDEX(_xlfn.TEXTSPLIT(C8, "-"), 1)</f>
         <v>nominal</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L8" s="3">
         <v>0</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N8" s="3">
         <v>50</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="P8" s="2" t="b">
         <v>1</v>
@@ -1201,17 +1195,17 @@
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" s="2" t="str" cm="1">
         <f t="array" ref="D9">INDEX(_xlfn.TEXTSPLIT(C9, "-"), 1)</f>
         <v>numeric</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
@@ -1230,13 +1224,13 @@
         <v>0</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N9" s="3">
         <v>0</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P9" s="2" t="b">
         <v>1</v>
@@ -1267,36 +1261,36 @@
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D10" s="2" t="str" cm="1">
         <f t="array" ref="D10">INDEX(_xlfn.TEXTSPLIT(C10, "-"), 1)</f>
         <v>nominal</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L10" s="3">
         <v>0</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N10" s="3">
         <v>0</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P10" s="2" t="b">
         <v>1</v>
@@ -1327,17 +1321,17 @@
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="str" cm="1">
         <f t="array" ref="D11">INDEX(_xlfn.TEXTSPLIT(C11, "-"), 1)</f>
         <v>numeric</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
@@ -1356,13 +1350,13 @@
         <v>0</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N11" s="3">
         <v>0</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P11" s="2" t="b">
         <v>1</v>
@@ -1393,36 +1387,36 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2" t="str" cm="1">
         <f t="array" ref="D12">INDEX(_xlfn.TEXTSPLIT(C12, "-"), 1)</f>
         <v>nominal</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L12" s="3">
         <v>0</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N12" s="3">
         <v>0</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P12" s="2" t="b">
         <v>1</v>
@@ -1453,36 +1447,36 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" s="2" t="str" cm="1">
         <f t="array" ref="D13">INDEX(_xlfn.TEXTSPLIT(C13, "-"), 1)</f>
         <v>nominal</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L13" s="3">
         <v>0</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N13" s="3">
         <v>0</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P13" s="2" t="b">
         <v>1</v>
@@ -23916,7 +23910,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -23944,13 +23938,13 @@
         <v>37</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>38</v>
@@ -23959,19 +23953,19 @@
         <v>40</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>41</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>42</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>15</v>
@@ -23992,7 +23986,7 @@
         <v>35</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="U1" s="8" t="s">
         <v>36</v>
@@ -24023,10 +24017,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
@@ -24034,19 +24028,19 @@
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J2" s="3">
         <v>0</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L2" s="3">
         <v>50</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N2" s="2" t="b">
         <v>1</v>
@@ -24079,17 +24073,17 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>46</v>
@@ -24098,13 +24092,13 @@
         <v>0</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L3" s="3">
         <v>6</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N3" s="2" t="b">
         <v>1</v>
@@ -24137,17 +24131,17 @@
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>46</v>
@@ -24156,13 +24150,13 @@
         <v>0</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L4" s="3">
         <v>4</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N4" s="2" t="b">
         <v>1</v>
@@ -24195,17 +24189,17 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>45</v>
@@ -24214,13 +24208,13 @@
         <v>0</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L5" s="3">
         <v>0</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N5" s="2" t="b">
         <v>1</v>
@@ -24253,17 +24247,17 @@
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>45</v>
@@ -24272,13 +24266,13 @@
         <v>0</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L6" s="3">
         <v>0</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N6" s="2" t="b">
         <v>1</v>
@@ -46221,7 +46215,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="15" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
better state validation in excel
</commit_message>
<xml_diff>
--- a/taks.xlsx
+++ b/taks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaha\Projects\Python Projects\TAKAutomator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C3AEE5-A786-4EFB-ABF0-A8A2D0809212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A0AD71-41E5-4B1B-9FF9-337E4BD46569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_concepts" sheetId="1" r:id="rId1"/>
@@ -794,7 +794,7 @@
   </sheetPr>
   <dimension ref="A1:W904"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
@@ -24031,9 +24031,9 @@
   </sheetPr>
   <dimension ref="A1:AI995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding no duplicated TAK_NAME validation
</commit_message>
<xml_diff>
--- a/taks.xlsx
+++ b/taks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonat\CodeProjects\TAKAutomator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7119EB61-9C3F-4002-A5D5-41EAB065579B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD375DA8-B1BA-429E-BC20-7980D5EA2600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_concepts" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">raw_concepts!$A$1:$T$908</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="m83MNRr2xD5s28t3NAVNceEtqFMD8kPYDDFbaPOQWh4="/>
     </ext>
@@ -33,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="297">
   <si>
     <t>TYPE</t>
   </si>
@@ -832,6 +843,99 @@
   <si>
     <t>["Normal", "Borderline", "Mild", "Marked"]</t>
   </si>
+  <si>
+    <t>ASPIRIN_BITZUA_EVENT</t>
+  </si>
+  <si>
+    <t>NITROGLYCERIN_BITZUA_EVENT</t>
+  </si>
+  <si>
+    <t>CLOPIDOGREL_BITZUA_EVENT</t>
+  </si>
+  <si>
+    <t>HEPARIN_BITZUA_EVENT</t>
+  </si>
+  <si>
+    <t>SODIUM_BITZUA_EVENT</t>
+  </si>
+  <si>
+    <t>ADMISSION_EVENT</t>
+  </si>
+  <si>
+    <t>RELEASE_EVENT</t>
+  </si>
+  <si>
+    <t>MEAL_EVENT</t>
+  </si>
+  <si>
+    <t>DEATH_EVENT</t>
+  </si>
+  <si>
+    <t>KETOACIDOSIS_EVENT</t>
+  </si>
+  <si>
+    <t>KIDNEY_DISORDER_EVENT</t>
+  </si>
+  <si>
+    <t>COMA_EVENT</t>
+  </si>
+  <si>
+    <t>EYE_DISORDER_EVENT</t>
+  </si>
+  <si>
+    <t>NERVOUS_SYSTEM_DISORDER_EVENT</t>
+  </si>
+  <si>
+    <t>VASCULAR_DISORDER_EVENT</t>
+  </si>
+  <si>
+    <t>OTHER_COMPLICATION_EVENT</t>
+  </si>
+  <si>
+    <t>DEMENTIA_EVENT</t>
+  </si>
+  <si>
+    <t>CARDIOVASCULAR_DISORDER_EVENT</t>
+  </si>
+  <si>
+    <t>ULCER_EVENT</t>
+  </si>
+  <si>
+    <t>INFECTIONS_EVENT</t>
+  </si>
+  <si>
+    <t>MUSCULOSKELETAL_COMPLICATION_EVENT</t>
+  </si>
+  <si>
+    <t>NEUROVASCULAR_COMPLICATION_EVENT</t>
+  </si>
+  <si>
+    <t>DIABETES_DIAGNOSIS_CONTEXT</t>
+  </si>
+  <si>
+    <t>UNEXPECTED_FALLS_CONTEXT</t>
+  </si>
+  <si>
+    <t>ALCOHOL_ABUSE_CONTEXT</t>
+  </si>
+  <si>
+    <t>CANCER_DIAGNOSIS_CONTEXT</t>
+  </si>
+  <si>
+    <t>BYPASS_CONTEXT</t>
+  </si>
+  <si>
+    <t>CREATINE-KINASE_MEASURE_STATE</t>
+  </si>
+  <si>
+    <t>CHOLESTEROL_MEASURE_STATE</t>
+  </si>
+  <si>
+    <t>TROPONIN_SERUM_MEASURE_STATE</t>
+  </si>
+  <si>
+    <t>TROPONIN_BLOOD_MEASURE_STATE</t>
+  </si>
 </sst>
 </file>
 
@@ -1323,8 +1427,8 @@
   <dimension ref="A1:T908"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24252,9 +24356,9 @@
   </sheetPr>
   <dimension ref="A1:AF994"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -26400,7 +26504,7 @@
         <v>1064</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>251</v>
+        <v>293</v>
       </c>
       <c r="C40" s="3">
         <v>64</v>
@@ -26454,7 +26558,7 @@
         <v>1065</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>252</v>
+        <v>294</v>
       </c>
       <c r="C41" s="3">
         <v>65</v>
@@ -26508,7 +26612,7 @@
         <v>1066</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>253</v>
+        <v>295</v>
       </c>
       <c r="C42" s="3">
         <v>66</v>
@@ -26562,7 +26666,7 @@
         <v>1067</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>254</v>
+        <v>296</v>
       </c>
       <c r="C43" s="3">
         <v>67</v>
@@ -44711,8 +44815,8 @@
   <dimension ref="A1:X1017"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -45190,7 +45294,7 @@
         <v>1183</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="C14" s="3">
         <v>83</v>
@@ -45224,7 +45328,7 @@
         <v>1184</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="C15" s="3">
         <v>84</v>
@@ -45258,7 +45362,7 @@
         <v>1185</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="C16" s="3">
         <v>85</v>
@@ -45292,7 +45396,7 @@
         <v>1186</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="C17" s="3">
         <v>86</v>
@@ -45326,7 +45430,7 @@
         <v>1187</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="C18" s="3">
         <v>87</v>
@@ -45360,7 +45464,7 @@
         <v>1111</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>1</v>
+        <v>271</v>
       </c>
       <c r="C19" s="3">
         <v>11</v>
@@ -45394,7 +45498,7 @@
         <v>1112</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>113</v>
+        <v>272</v>
       </c>
       <c r="C20" s="3">
         <v>12</v>
@@ -45428,7 +45532,7 @@
         <v>1110</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>11</v>
+        <v>273</v>
       </c>
       <c r="C21" s="3">
         <v>10</v>
@@ -45462,7 +45566,7 @@
         <v>1108</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>2</v>
+        <v>274</v>
       </c>
       <c r="C22" s="3">
         <v>8</v>
@@ -45496,7 +45600,7 @@
         <v>1109</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>111</v>
+        <v>275</v>
       </c>
       <c r="C23" s="3">
         <v>9</v>
@@ -45530,7 +45634,7 @@
         <v>1113</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>114</v>
+        <v>276</v>
       </c>
       <c r="C24" s="3">
         <v>13</v>
@@ -45564,7 +45668,7 @@
         <v>1114</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>112</v>
+        <v>277</v>
       </c>
       <c r="C25" s="3">
         <v>14</v>
@@ -45598,7 +45702,7 @@
         <v>1115</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>120</v>
+        <v>278</v>
       </c>
       <c r="C26" s="3">
         <v>15</v>
@@ -45632,7 +45736,7 @@
         <v>1116</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>121</v>
+        <v>279</v>
       </c>
       <c r="C27" s="3">
         <v>16</v>
@@ -45666,7 +45770,7 @@
         <v>1117</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>122</v>
+        <v>280</v>
       </c>
       <c r="C28" s="3">
         <v>17</v>
@@ -45700,7 +45804,7 @@
         <v>1118</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
       <c r="C29" s="3">
         <v>18</v>
@@ -45734,7 +45838,7 @@
         <v>1119</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>124</v>
+        <v>282</v>
       </c>
       <c r="C30" s="3">
         <v>19</v>
@@ -45768,7 +45872,7 @@
         <v>1120</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>125</v>
+        <v>283</v>
       </c>
       <c r="C31" s="3">
         <v>20</v>
@@ -45802,7 +45906,7 @@
         <v>1121</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>126</v>
+        <v>284</v>
       </c>
       <c r="C32" s="3">
         <v>21</v>
@@ -45836,7 +45940,7 @@
         <v>1122</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>127</v>
+        <v>285</v>
       </c>
       <c r="C33" s="3">
         <v>22</v>
@@ -45870,7 +45974,7 @@
         <v>1123</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>128</v>
+        <v>286</v>
       </c>
       <c r="C34" s="3">
         <v>23</v>
@@ -45904,7 +46008,7 @@
         <v>1124</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>129</v>
+        <v>287</v>
       </c>
       <c r="C35" s="3">
         <v>24</v>
@@ -58720,9 +58824,9 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -58830,7 +58934,7 @@
         <v>1203</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>288</v>
       </c>
       <c r="C2" s="19">
         <v>3</v>
@@ -58882,7 +58986,7 @@
         <v>1225</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>130</v>
+        <v>289</v>
       </c>
       <c r="C3" s="3">
         <v>25</v>
@@ -58926,7 +59030,7 @@
         <v>1226</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>131</v>
+        <v>290</v>
       </c>
       <c r="C4" s="23">
         <v>26</v>
@@ -58970,7 +59074,7 @@
         <v>1227</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>132</v>
+        <v>291</v>
       </c>
       <c r="C5" s="23">
         <v>27</v>
@@ -59014,7 +59118,7 @@
         <v>1228</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>258</v>
+        <v>292</v>
       </c>
       <c r="C6" s="23">
         <v>28</v>

</xml_diff>

<commit_message>
adding functionality to handle nominal based states
</commit_message>
<xml_diff>
--- a/taks.xlsx
+++ b/taks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonat\CodeProjects\TAKAutomator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E4FDF1-F2E4-4014-9372-DBE4567B3000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C36AB59-D9CE-4E03-BC63-93CF2C7DF5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_concepts" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="310">
   <si>
     <t>TYPE</t>
   </si>
@@ -966,6 +966,15 @@
   <si>
     <t>MENTAL_HEALTH_MEDS_BITZUA_EVENT</t>
   </si>
+  <si>
+    <t>STEROIDS_DOSAGE_STATE</t>
+  </si>
+  <si>
+    <t>ANTIDIABETIC_DRUGS_IV_DOSAGE_STATE</t>
+  </si>
+  <si>
+    <t>ANTIDIABETIC_DRUGS_PO_DOSAGE_STATE</t>
+  </si>
 </sst>
 </file>
 
@@ -1023,7 +1032,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1033,12 +1042,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,7 +1111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1211,6 +1214,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1218,23 +1224,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1456,9 +1446,9 @@
   </sheetPr>
   <dimension ref="A1:T908"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1600,58 +1590,58 @@
       </c>
       <c r="T2" s="4"/>
     </row>
-    <row r="3" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41">
+    <row r="3" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36">
         <v>6</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="42" t="str">
+      <c r="D3" s="37" t="str">
         <f t="shared" si="0"/>
         <v>nominal</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="41" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="41">
+      <c r="J3" s="36">
         <v>0</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="41">
+      <c r="L3" s="36">
         <v>24</v>
       </c>
-      <c r="M3" s="41" t="s">
+      <c r="M3" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O3" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P3" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q3" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R3" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S3" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T3" s="45" t="s">
+      <c r="N3" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R3" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3" s="40" t="s">
         <v>260</v>
       </c>
     </row>
@@ -1714,58 +1704,58 @@
       </c>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41">
+    <row r="5" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="36">
         <v>7</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="42" t="str">
+      <c r="D5" s="37" t="str">
         <f t="shared" ref="D5" si="1">LEFT(C5, FIND("-", C5)-1)</f>
         <v>nominal</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="41">
+      <c r="J5" s="36">
         <v>0</v>
       </c>
-      <c r="K5" s="41" t="s">
+      <c r="K5" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L5" s="41">
+      <c r="L5" s="36">
         <v>8</v>
       </c>
-      <c r="M5" s="41" t="s">
+      <c r="M5" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N5" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P5" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q5" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R5" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S5" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T5" s="45" t="s">
+      <c r="N5" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S5" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T5" s="40" t="s">
         <v>260</v>
       </c>
     </row>
@@ -1873,7 +1863,7 @@
       <c r="S7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="T7" s="48"/>
+      <c r="T7" s="43"/>
     </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -2403,7 +2393,7 @@
       <c r="S17" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="T17" s="48"/>
+      <c r="T17" s="43"/>
     </row>
     <row r="18" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -2456,7 +2446,7 @@
       <c r="S18" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="T18" s="48"/>
+      <c r="T18" s="43"/>
     </row>
     <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -2723,111 +2713,111 @@
       </c>
       <c r="T23" s="4"/>
     </row>
-    <row r="24" spans="1:20" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31">
+    <row r="24" spans="1:20" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="25">
         <v>10</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="32" t="str">
+      <c r="D24" s="27" t="str">
         <f t="shared" si="0"/>
         <v>nominal</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31" t="s">
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J24" s="31">
+      <c r="J24" s="25">
         <v>0</v>
       </c>
-      <c r="K24" s="31" t="s">
+      <c r="K24" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="L24" s="31">
+      <c r="L24" s="25">
         <v>0</v>
       </c>
-      <c r="M24" s="31" t="s">
+      <c r="M24" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="N24" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="O24" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="P24" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q24" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="R24" s="33" t="s">
+      <c r="N24" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="O24" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="P24" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q24" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="R24" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="S24" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="T24" s="34"/>
-    </row>
-    <row r="25" spans="1:20" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="31">
+      <c r="S24" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="T24" s="29"/>
+    </row>
+    <row r="25" spans="1:20" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="25">
         <v>11</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="32" t="str">
+      <c r="D25" s="27" t="str">
         <f>LEFT(C25, FIND("-", C25)-1)</f>
         <v>nominal</v>
       </c>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="31" t="s">
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="31">
+      <c r="J25" s="25">
         <v>0</v>
       </c>
-      <c r="K25" s="31" t="s">
+      <c r="K25" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="L25" s="31">
+      <c r="L25" s="25">
         <v>0</v>
       </c>
-      <c r="M25" s="31" t="s">
+      <c r="M25" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="N25" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="O25" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="P25" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q25" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="R25" s="33" t="s">
+      <c r="N25" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="O25" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="P25" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q25" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="R25" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="S25" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="T25" s="34"/>
+      <c r="S25" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="T25" s="29"/>
     </row>
     <row r="26" spans="1:20" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
@@ -3624,2627 +3614,2627 @@
       </c>
       <c r="T40" s="29"/>
     </row>
-    <row r="41" spans="1:20" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="36">
+    <row r="41" spans="1:20" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="31">
         <v>3</v>
       </c>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C41" s="37" t="s">
+      <c r="C41" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D41" s="37" t="str">
+      <c r="D41" s="32" t="str">
         <f t="shared" ref="D41" si="9">LEFT(C41, FIND("-", C41)-1)</f>
         <v>nominal</v>
       </c>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="36" t="s">
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="J41" s="36">
+      <c r="J41" s="31">
         <v>0</v>
       </c>
-      <c r="K41" s="36" t="s">
+      <c r="K41" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="L41" s="36">
+      <c r="L41" s="31">
         <v>1</v>
       </c>
-      <c r="M41" s="36" t="s">
+      <c r="M41" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="N41" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="O41" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="P41" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q41" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="R41" s="38" t="s">
+      <c r="N41" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="O41" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="P41" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q41" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="R41" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="S41" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="T41" s="39"/>
-    </row>
-    <row r="42" spans="1:20" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="36">
+      <c r="S41" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="T41" s="34"/>
+    </row>
+    <row r="42" spans="1:20" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="31">
         <v>25</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="37" t="str">
+      <c r="D42" s="32" t="str">
         <f>LEFT(C42, FIND("-", C42)-1)</f>
         <v>nominal</v>
       </c>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="36" t="s">
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="J42" s="36">
+      <c r="J42" s="31">
         <v>0</v>
       </c>
-      <c r="K42" s="36" t="s">
+      <c r="K42" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="L42" s="36">
+      <c r="L42" s="31">
         <v>1</v>
       </c>
-      <c r="M42" s="36" t="s">
+      <c r="M42" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="N42" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="O42" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="P42" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q42" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="R42" s="38" t="s">
+      <c r="N42" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="O42" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="P42" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q42" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="R42" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="S42" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="T42" s="39"/>
-    </row>
-    <row r="43" spans="1:20" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="36">
+      <c r="S42" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="T42" s="34"/>
+    </row>
+    <row r="43" spans="1:20" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="31">
         <v>26</v>
       </c>
-      <c r="B43" s="37" t="s">
+      <c r="B43" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="37" t="s">
+      <c r="C43" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D43" s="37" t="str">
+      <c r="D43" s="32" t="str">
         <f>LEFT(C43, FIND("-", C43)-1)</f>
         <v>nominal</v>
       </c>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="36" t="s">
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="J43" s="36">
+      <c r="J43" s="31">
         <v>0</v>
       </c>
-      <c r="K43" s="36" t="s">
+      <c r="K43" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="L43" s="36">
+      <c r="L43" s="31">
         <v>1</v>
       </c>
-      <c r="M43" s="36" t="s">
+      <c r="M43" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="N43" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="O43" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="P43" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q43" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="R43" s="38" t="s">
+      <c r="N43" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="O43" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="P43" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q43" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="R43" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="S43" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="T43" s="39"/>
-    </row>
-    <row r="44" spans="1:20" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="36">
+      <c r="S43" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="T43" s="34"/>
+    </row>
+    <row r="44" spans="1:20" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="31">
         <v>27</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C44" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D44" s="37" t="str">
+      <c r="D44" s="32" t="str">
         <f>LEFT(C44, FIND("-", C44)-1)</f>
         <v>nominal</v>
       </c>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="36" t="s">
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="J44" s="36">
+      <c r="J44" s="31">
         <v>0</v>
       </c>
-      <c r="K44" s="36" t="s">
+      <c r="K44" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="L44" s="36">
+      <c r="L44" s="31">
         <v>1</v>
       </c>
-      <c r="M44" s="36" t="s">
+      <c r="M44" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="N44" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="O44" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="P44" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q44" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="R44" s="38" t="s">
+      <c r="N44" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="O44" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="P44" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q44" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="R44" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="S44" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="T44" s="39"/>
-    </row>
-    <row r="45" spans="1:20" s="40" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="36">
+      <c r="S44" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="T44" s="34"/>
+    </row>
+    <row r="45" spans="1:20" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="31">
         <v>28</v>
       </c>
-      <c r="B45" s="37" t="s">
+      <c r="B45" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="C45" s="37" t="s">
+      <c r="C45" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D45" s="37" t="str">
+      <c r="D45" s="32" t="str">
         <f>LEFT(C45, FIND("-", C45)-1)</f>
         <v>nominal</v>
       </c>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="36" t="s">
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="J45" s="36">
+      <c r="J45" s="31">
         <v>0</v>
       </c>
-      <c r="K45" s="36" t="s">
+      <c r="K45" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="L45" s="36">
+      <c r="L45" s="31">
         <v>1</v>
       </c>
-      <c r="M45" s="36" t="s">
+      <c r="M45" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="N45" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="O45" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="P45" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q45" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="R45" s="38" t="s">
+      <c r="N45" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="O45" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="P45" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q45" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="R45" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="S45" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="T45" s="39"/>
-    </row>
-    <row r="46" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="41">
+      <c r="S45" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="T45" s="34"/>
+    </row>
+    <row r="46" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="36">
         <v>1</v>
       </c>
-      <c r="B46" s="42" t="s">
+      <c r="B46" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C46" s="42" t="s">
+      <c r="C46" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="42" t="str">
+      <c r="D46" s="37" t="str">
         <f t="shared" ref="D46:D47" si="10">LEFT(C46, FIND("-", C46)-1)</f>
         <v>numeric</v>
       </c>
-      <c r="E46" s="42">
+      <c r="E46" s="37">
         <v>0</v>
       </c>
-      <c r="F46" s="43">
+      <c r="F46" s="38">
         <v>800</v>
       </c>
-      <c r="G46" s="43" t="s">
+      <c r="G46" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="I46" s="42"/>
-      <c r="J46" s="41">
+      <c r="I46" s="37"/>
+      <c r="J46" s="36">
         <v>0</v>
       </c>
-      <c r="K46" s="41" t="s">
+      <c r="K46" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L46" s="41">
+      <c r="L46" s="36">
         <v>6</v>
       </c>
-      <c r="M46" s="41" t="s">
+      <c r="M46" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N46" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O46" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P46" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q46" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R46" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S46" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T46" s="45"/>
-    </row>
-    <row r="47" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="41">
+      <c r="N46" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O46" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P46" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q46" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R46" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S46" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T46" s="40"/>
+    </row>
+    <row r="47" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="36">
         <v>2</v>
       </c>
-      <c r="B47" s="42" t="s">
+      <c r="B47" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="42" t="s">
+      <c r="C47" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="42" t="str">
+      <c r="D47" s="37" t="str">
         <f t="shared" si="10"/>
         <v>numeric</v>
       </c>
-      <c r="E47" s="42">
+      <c r="E47" s="37">
         <v>0</v>
       </c>
-      <c r="F47" s="43">
+      <c r="F47" s="38">
         <v>600</v>
       </c>
-      <c r="G47" s="43" t="s">
+      <c r="G47" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H47" s="43" t="s">
+      <c r="H47" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="I47" s="42"/>
-      <c r="J47" s="42">
+      <c r="I47" s="37"/>
+      <c r="J47" s="37">
         <v>0</v>
       </c>
-      <c r="K47" s="41" t="s">
+      <c r="K47" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L47" s="42">
+      <c r="L47" s="37">
         <v>4</v>
       </c>
-      <c r="M47" s="41" t="s">
+      <c r="M47" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N47" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O47" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P47" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q47" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R47" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S47" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T47" s="45"/>
-    </row>
-    <row r="48" spans="1:20" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="41">
+      <c r="N47" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O47" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P47" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q47" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R47" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S47" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T47" s="40"/>
+    </row>
+    <row r="48" spans="1:20" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="36">
         <v>30</v>
       </c>
-      <c r="B48" s="41" t="s">
+      <c r="B48" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="C48" s="42" t="s">
+      <c r="C48" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D48" s="42" t="str">
+      <c r="D48" s="37" t="str">
         <f t="shared" si="0"/>
         <v>numeric</v>
       </c>
-      <c r="E48" s="42">
+      <c r="E48" s="37">
         <v>0</v>
       </c>
-      <c r="F48" s="41">
+      <c r="F48" s="36">
         <v>100</v>
       </c>
-      <c r="G48" s="42" t="s">
+      <c r="G48" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="H48" s="41" t="s">
+      <c r="H48" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I48" s="41"/>
-      <c r="J48" s="41">
+      <c r="I48" s="36"/>
+      <c r="J48" s="36">
         <v>0</v>
       </c>
-      <c r="K48" s="41" t="s">
+      <c r="K48" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L48" s="41">
+      <c r="L48" s="36">
         <v>24</v>
       </c>
-      <c r="M48" s="41" t="s">
+      <c r="M48" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N48" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O48" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P48" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q48" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R48" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S48" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T48" s="45"/>
-    </row>
-    <row r="49" spans="1:20" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="41">
+      <c r="N48" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O48" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P48" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q48" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R48" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S48" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T48" s="40"/>
+    </row>
+    <row r="49" spans="1:20" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="36">
         <v>31</v>
       </c>
-      <c r="B49" s="41" t="s">
+      <c r="B49" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="C49" s="42" t="s">
+      <c r="C49" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D49" s="42" t="str">
+      <c r="D49" s="37" t="str">
         <f t="shared" ref="D49:D81" si="11">LEFT(C49, FIND("-", C49)-1)</f>
         <v>numeric</v>
       </c>
-      <c r="E49" s="42">
+      <c r="E49" s="37">
         <v>0</v>
       </c>
-      <c r="F49" s="41">
+      <c r="F49" s="36">
         <v>6</v>
       </c>
-      <c r="G49" s="42" t="s">
+      <c r="G49" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="H49" s="41" t="s">
+      <c r="H49" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I49" s="41"/>
-      <c r="J49" s="41">
+      <c r="I49" s="36"/>
+      <c r="J49" s="36">
         <v>0</v>
       </c>
-      <c r="K49" s="41" t="s">
+      <c r="K49" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L49" s="41">
+      <c r="L49" s="36">
         <v>24</v>
       </c>
-      <c r="M49" s="41" t="s">
+      <c r="M49" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N49" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O49" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P49" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q49" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R49" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S49" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T49" s="45"/>
-    </row>
-    <row r="50" spans="1:20" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="41">
+      <c r="N49" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O49" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P49" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q49" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R49" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S49" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T49" s="40"/>
+    </row>
+    <row r="50" spans="1:20" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="36">
         <v>32</v>
       </c>
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="C50" s="42" t="s">
+      <c r="C50" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D50" s="42" t="str">
+      <c r="D50" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E50" s="42">
+      <c r="E50" s="37">
         <v>0</v>
       </c>
-      <c r="F50" s="41">
+      <c r="F50" s="36">
         <v>15</v>
       </c>
-      <c r="G50" s="42" t="s">
+      <c r="G50" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="H50" s="41" t="s">
+      <c r="H50" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I50" s="41"/>
-      <c r="J50" s="41">
+      <c r="I50" s="36"/>
+      <c r="J50" s="36">
         <v>0</v>
       </c>
-      <c r="K50" s="41" t="s">
+      <c r="K50" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L50" s="41">
+      <c r="L50" s="36">
         <v>2</v>
       </c>
-      <c r="M50" s="41" t="s">
+      <c r="M50" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="N50" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O50" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P50" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q50" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R50" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S50" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T50" s="45"/>
-    </row>
-    <row r="51" spans="1:20" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="41">
+      <c r="N50" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O50" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P50" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q50" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R50" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S50" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T50" s="40"/>
+    </row>
+    <row r="51" spans="1:20" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="36">
         <v>33</v>
       </c>
-      <c r="B51" s="41" t="s">
+      <c r="B51" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="C51" s="42" t="s">
+      <c r="C51" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D51" s="42" t="str">
+      <c r="D51" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E51" s="42">
+      <c r="E51" s="37">
         <v>0</v>
       </c>
-      <c r="F51" s="41">
+      <c r="F51" s="36">
         <v>100</v>
       </c>
-      <c r="G51" s="42" t="s">
+      <c r="G51" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="H51" s="41" t="s">
+      <c r="H51" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I51" s="41"/>
-      <c r="J51" s="41">
+      <c r="I51" s="36"/>
+      <c r="J51" s="36">
         <v>0</v>
       </c>
-      <c r="K51" s="41" t="s">
+      <c r="K51" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L51" s="41">
+      <c r="L51" s="36">
         <v>24</v>
       </c>
-      <c r="M51" s="41" t="s">
+      <c r="M51" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N51" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O51" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P51" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q51" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R51" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S51" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T51" s="45"/>
-    </row>
-    <row r="52" spans="1:20" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="41">
+      <c r="N51" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O51" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P51" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q51" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R51" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S51" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T51" s="40"/>
+    </row>
+    <row r="52" spans="1:20" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="36">
         <v>34</v>
       </c>
-      <c r="B52" s="41" t="s">
+      <c r="B52" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="42" t="s">
+      <c r="C52" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D52" s="42" t="str">
+      <c r="D52" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E52" s="42">
+      <c r="E52" s="37">
         <v>0</v>
       </c>
-      <c r="F52" s="41">
+      <c r="F52" s="36">
         <v>200</v>
       </c>
-      <c r="G52" s="42" t="s">
+      <c r="G52" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="H52" s="41" t="s">
+      <c r="H52" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I52" s="41"/>
-      <c r="J52" s="41">
+      <c r="I52" s="36"/>
+      <c r="J52" s="36">
         <v>0</v>
       </c>
-      <c r="K52" s="41" t="s">
+      <c r="K52" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L52" s="41">
+      <c r="L52" s="36">
         <v>24</v>
       </c>
-      <c r="M52" s="41" t="s">
+      <c r="M52" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N52" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O52" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P52" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q52" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R52" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S52" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T52" s="45"/>
-    </row>
-    <row r="53" spans="1:20" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="41">
+      <c r="N52" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O52" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P52" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q52" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R52" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S52" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T52" s="40"/>
+    </row>
+    <row r="53" spans="1:20" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="36">
         <v>35</v>
       </c>
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="C53" s="42" t="s">
+      <c r="C53" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D53" s="42" t="str">
+      <c r="D53" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E53" s="42">
+      <c r="E53" s="37">
         <v>0</v>
       </c>
-      <c r="F53" s="41">
+      <c r="F53" s="36">
         <v>100</v>
       </c>
-      <c r="G53" s="42" t="s">
+      <c r="G53" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="H53" s="41" t="s">
+      <c r="H53" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I53" s="41"/>
-      <c r="J53" s="41">
+      <c r="I53" s="36"/>
+      <c r="J53" s="36">
         <v>0</v>
       </c>
-      <c r="K53" s="41" t="s">
+      <c r="K53" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L53" s="41">
+      <c r="L53" s="36">
         <v>24</v>
       </c>
-      <c r="M53" s="41" t="s">
+      <c r="M53" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N53" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O53" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P53" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q53" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R53" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S53" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T53" s="45"/>
-    </row>
-    <row r="54" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="41">
+      <c r="N53" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O53" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P53" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q53" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R53" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S53" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T53" s="40"/>
+    </row>
+    <row r="54" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="36">
         <v>36</v>
       </c>
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="C54" s="42" t="s">
+      <c r="C54" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D54" s="42" t="str">
+      <c r="D54" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E54" s="42">
+      <c r="E54" s="37">
         <v>0</v>
       </c>
-      <c r="F54" s="41">
+      <c r="F54" s="36">
         <v>100</v>
       </c>
-      <c r="G54" s="43" t="s">
+      <c r="G54" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H54" s="41" t="s">
+      <c r="H54" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I54" s="41"/>
-      <c r="J54" s="41">
+      <c r="I54" s="36"/>
+      <c r="J54" s="36">
         <v>0</v>
       </c>
-      <c r="K54" s="41" t="s">
+      <c r="K54" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L54" s="41">
+      <c r="L54" s="36">
         <v>24</v>
       </c>
-      <c r="M54" s="41" t="s">
+      <c r="M54" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N54" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O54" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P54" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q54" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R54" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S54" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T54" s="45"/>
-    </row>
-    <row r="55" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="41">
+      <c r="N54" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O54" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P54" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q54" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R54" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S54" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T54" s="40"/>
+    </row>
+    <row r="55" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="36">
         <v>37</v>
       </c>
-      <c r="B55" s="41" t="s">
+      <c r="B55" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="C55" s="42" t="s">
+      <c r="C55" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D55" s="42" t="str">
+      <c r="D55" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E55" s="42">
+      <c r="E55" s="37">
         <v>0</v>
       </c>
-      <c r="F55" s="41">
+      <c r="F55" s="36">
         <v>100</v>
       </c>
-      <c r="G55" s="43" t="s">
+      <c r="G55" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H55" s="41" t="s">
+      <c r="H55" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I55" s="41"/>
-      <c r="J55" s="41">
+      <c r="I55" s="36"/>
+      <c r="J55" s="36">
         <v>0</v>
       </c>
-      <c r="K55" s="41" t="s">
+      <c r="K55" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L55" s="41">
+      <c r="L55" s="36">
         <v>24</v>
       </c>
-      <c r="M55" s="41" t="s">
+      <c r="M55" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N55" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O55" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P55" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q55" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R55" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S55" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T55" s="45"/>
-    </row>
-    <row r="56" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="41">
+      <c r="N55" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O55" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P55" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q55" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R55" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S55" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T55" s="40"/>
+    </row>
+    <row r="56" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="36">
         <v>38</v>
       </c>
-      <c r="B56" s="41" t="s">
+      <c r="B56" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="42" t="s">
+      <c r="C56" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D56" s="42" t="str">
+      <c r="D56" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E56" s="42">
+      <c r="E56" s="37">
         <v>0</v>
       </c>
-      <c r="F56" s="41">
+      <c r="F56" s="36">
         <v>100</v>
       </c>
-      <c r="G56" s="43" t="s">
+      <c r="G56" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H56" s="41" t="s">
+      <c r="H56" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I56" s="41"/>
-      <c r="J56" s="41">
+      <c r="I56" s="36"/>
+      <c r="J56" s="36">
         <v>0</v>
       </c>
-      <c r="K56" s="41" t="s">
+      <c r="K56" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L56" s="41">
+      <c r="L56" s="36">
         <v>24</v>
       </c>
-      <c r="M56" s="41" t="s">
+      <c r="M56" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N56" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O56" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P56" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q56" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R56" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S56" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T56" s="45"/>
-    </row>
-    <row r="57" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="41">
+      <c r="N56" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O56" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P56" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q56" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R56" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S56" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T56" s="40"/>
+    </row>
+    <row r="57" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="36">
         <v>39</v>
       </c>
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="C57" s="42" t="s">
+      <c r="C57" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="42" t="str">
+      <c r="D57" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E57" s="42">
+      <c r="E57" s="37">
         <v>0</v>
       </c>
-      <c r="F57" s="41">
+      <c r="F57" s="36">
         <v>100</v>
       </c>
-      <c r="G57" s="43" t="s">
+      <c r="G57" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H57" s="41" t="s">
+      <c r="H57" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I57" s="41"/>
-      <c r="J57" s="41">
+      <c r="I57" s="36"/>
+      <c r="J57" s="36">
         <v>0</v>
       </c>
-      <c r="K57" s="41" t="s">
+      <c r="K57" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L57" s="41">
+      <c r="L57" s="36">
         <v>24</v>
       </c>
-      <c r="M57" s="41" t="s">
+      <c r="M57" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N57" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O57" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P57" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q57" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R57" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S57" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T57" s="45"/>
-    </row>
-    <row r="58" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="41">
+      <c r="N57" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O57" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P57" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q57" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R57" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S57" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T57" s="40"/>
+    </row>
+    <row r="58" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="36">
         <v>40</v>
       </c>
-      <c r="B58" s="41" t="s">
+      <c r="B58" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="C58" s="42" t="s">
+      <c r="C58" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D58" s="42" t="str">
+      <c r="D58" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E58" s="42">
+      <c r="E58" s="37">
         <v>0</v>
       </c>
-      <c r="F58" s="41">
+      <c r="F58" s="36">
         <v>1000</v>
       </c>
-      <c r="G58" s="43" t="s">
+      <c r="G58" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H58" s="41" t="s">
+      <c r="H58" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I58" s="41"/>
-      <c r="J58" s="41">
+      <c r="I58" s="36"/>
+      <c r="J58" s="36">
         <v>0</v>
       </c>
-      <c r="K58" s="41" t="s">
+      <c r="K58" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L58" s="41">
+      <c r="L58" s="36">
         <v>24</v>
       </c>
-      <c r="M58" s="41" t="s">
+      <c r="M58" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N58" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O58" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P58" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q58" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R58" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S58" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T58" s="45"/>
-    </row>
-    <row r="59" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="41">
+      <c r="N58" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O58" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P58" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q58" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R58" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S58" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T58" s="40"/>
+    </row>
+    <row r="59" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="36">
         <v>41</v>
       </c>
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="C59" s="42" t="s">
+      <c r="C59" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D59" s="42" t="str">
+      <c r="D59" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E59" s="42">
+      <c r="E59" s="37">
         <v>0</v>
       </c>
-      <c r="F59" s="41">
+      <c r="F59" s="36">
         <v>100</v>
       </c>
-      <c r="G59" s="43" t="s">
+      <c r="G59" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H59" s="41" t="s">
+      <c r="H59" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I59" s="41"/>
-      <c r="J59" s="41">
+      <c r="I59" s="36"/>
+      <c r="J59" s="36">
         <v>0</v>
       </c>
-      <c r="K59" s="41" t="s">
+      <c r="K59" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L59" s="41">
+      <c r="L59" s="36">
         <v>24</v>
       </c>
-      <c r="M59" s="41" t="s">
+      <c r="M59" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N59" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O59" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P59" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q59" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R59" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S59" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T59" s="45"/>
-    </row>
-    <row r="60" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="41">
+      <c r="N59" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O59" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P59" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q59" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R59" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S59" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T59" s="40"/>
+    </row>
+    <row r="60" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="36">
         <v>42</v>
       </c>
-      <c r="B60" s="41" t="s">
+      <c r="B60" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C60" s="42" t="s">
+      <c r="C60" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D60" s="42" t="str">
+      <c r="D60" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E60" s="42">
+      <c r="E60" s="37">
         <v>0</v>
       </c>
-      <c r="F60" s="41">
+      <c r="F60" s="36">
         <v>100</v>
       </c>
-      <c r="G60" s="43" t="s">
+      <c r="G60" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H60" s="41" t="s">
+      <c r="H60" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I60" s="41"/>
-      <c r="J60" s="41">
+      <c r="I60" s="36"/>
+      <c r="J60" s="36">
         <v>0</v>
       </c>
-      <c r="K60" s="41" t="s">
+      <c r="K60" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L60" s="41">
+      <c r="L60" s="36">
         <v>24</v>
       </c>
-      <c r="M60" s="41" t="s">
+      <c r="M60" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N60" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O60" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P60" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q60" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R60" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S60" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T60" s="45"/>
-    </row>
-    <row r="61" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="41">
+      <c r="N60" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O60" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P60" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q60" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R60" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S60" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T60" s="40"/>
+    </row>
+    <row r="61" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="36">
         <v>43</v>
       </c>
-      <c r="B61" s="41" t="s">
+      <c r="B61" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C61" s="42" t="s">
+      <c r="C61" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D61" s="42" t="str">
+      <c r="D61" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E61" s="42">
+      <c r="E61" s="37">
         <v>0</v>
       </c>
-      <c r="F61" s="41">
+      <c r="F61" s="36">
         <v>100</v>
       </c>
-      <c r="G61" s="43" t="s">
+      <c r="G61" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H61" s="41" t="s">
+      <c r="H61" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I61" s="41"/>
-      <c r="J61" s="41">
+      <c r="I61" s="36"/>
+      <c r="J61" s="36">
         <v>0</v>
       </c>
-      <c r="K61" s="41" t="s">
+      <c r="K61" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L61" s="41">
+      <c r="L61" s="36">
         <v>24</v>
       </c>
-      <c r="M61" s="41" t="s">
+      <c r="M61" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N61" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O61" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P61" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q61" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R61" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S61" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T61" s="45"/>
-    </row>
-    <row r="62" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="41">
+      <c r="N61" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O61" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P61" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q61" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R61" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S61" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T61" s="40"/>
+    </row>
+    <row r="62" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="36">
         <v>44</v>
       </c>
-      <c r="B62" s="41" t="s">
+      <c r="B62" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="C62" s="42" t="s">
+      <c r="C62" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D62" s="42" t="str">
+      <c r="D62" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E62" s="42">
+      <c r="E62" s="37">
         <v>0</v>
       </c>
-      <c r="F62" s="41">
+      <c r="F62" s="36">
         <v>50000</v>
       </c>
-      <c r="G62" s="43" t="s">
+      <c r="G62" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H62" s="41" t="s">
+      <c r="H62" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I62" s="41"/>
-      <c r="J62" s="41">
+      <c r="I62" s="36"/>
+      <c r="J62" s="36">
         <v>0</v>
       </c>
-      <c r="K62" s="41" t="s">
+      <c r="K62" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L62" s="41">
+      <c r="L62" s="36">
         <v>24</v>
       </c>
-      <c r="M62" s="41" t="s">
+      <c r="M62" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N62" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O62" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P62" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q62" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R62" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S62" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T62" s="45"/>
-    </row>
-    <row r="63" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="41">
+      <c r="N62" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O62" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P62" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q62" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R62" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S62" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T62" s="40"/>
+    </row>
+    <row r="63" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="36">
         <v>45</v>
       </c>
-      <c r="B63" s="41" t="s">
+      <c r="B63" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="C63" s="42" t="s">
+      <c r="C63" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D63" s="42" t="str">
+      <c r="D63" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E63" s="42">
+      <c r="E63" s="37">
         <v>0</v>
       </c>
-      <c r="F63" s="41">
+      <c r="F63" s="36">
         <v>200</v>
       </c>
-      <c r="G63" s="43" t="s">
+      <c r="G63" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H63" s="41" t="s">
+      <c r="H63" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I63" s="41"/>
-      <c r="J63" s="41">
+      <c r="I63" s="36"/>
+      <c r="J63" s="36">
         <v>0</v>
       </c>
-      <c r="K63" s="41" t="s">
+      <c r="K63" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L63" s="41">
+      <c r="L63" s="36">
         <v>24</v>
       </c>
-      <c r="M63" s="41" t="s">
+      <c r="M63" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N63" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O63" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P63" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q63" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R63" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S63" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T63" s="45"/>
-    </row>
-    <row r="64" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="41">
+      <c r="N63" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O63" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P63" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q63" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R63" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S63" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T63" s="40"/>
+    </row>
+    <row r="64" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="36">
         <v>46</v>
       </c>
-      <c r="B64" s="41" t="s">
+      <c r="B64" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="C64" s="42" t="s">
+      <c r="C64" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D64" s="42" t="str">
+      <c r="D64" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E64" s="42">
+      <c r="E64" s="37">
         <v>0</v>
       </c>
-      <c r="F64" s="41">
+      <c r="F64" s="36">
         <v>100</v>
       </c>
-      <c r="G64" s="43" t="s">
+      <c r="G64" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H64" s="41" t="s">
+      <c r="H64" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I64" s="41"/>
-      <c r="J64" s="41">
+      <c r="I64" s="36"/>
+      <c r="J64" s="36">
         <v>0</v>
       </c>
-      <c r="K64" s="41" t="s">
+      <c r="K64" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L64" s="41">
+      <c r="L64" s="36">
         <v>14</v>
       </c>
-      <c r="M64" s="41" t="s">
+      <c r="M64" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="N64" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O64" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P64" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q64" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R64" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S64" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T64" s="45"/>
-    </row>
-    <row r="65" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="41">
+      <c r="N64" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O64" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P64" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q64" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R64" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S64" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T64" s="40"/>
+    </row>
+    <row r="65" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="36">
         <v>47</v>
       </c>
-      <c r="B65" s="41" t="s">
+      <c r="B65" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="C65" s="42" t="s">
+      <c r="C65" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D65" s="42" t="str">
+      <c r="D65" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E65" s="42">
+      <c r="E65" s="37">
         <v>0</v>
       </c>
-      <c r="F65" s="41">
+      <c r="F65" s="36">
         <v>10000</v>
       </c>
-      <c r="G65" s="43" t="s">
+      <c r="G65" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H65" s="41" t="s">
+      <c r="H65" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I65" s="41"/>
-      <c r="J65" s="41">
+      <c r="I65" s="36"/>
+      <c r="J65" s="36">
         <v>0</v>
       </c>
-      <c r="K65" s="41" t="s">
+      <c r="K65" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L65" s="41">
+      <c r="L65" s="36">
         <v>14</v>
       </c>
-      <c r="M65" s="41" t="s">
+      <c r="M65" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="N65" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O65" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P65" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q65" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R65" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S65" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T65" s="45"/>
-    </row>
-    <row r="66" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="41">
+      <c r="N65" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O65" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P65" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q65" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R65" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S65" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T65" s="40"/>
+    </row>
+    <row r="66" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="36">
         <v>48</v>
       </c>
-      <c r="B66" s="41" t="s">
+      <c r="B66" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="C66" s="42" t="s">
+      <c r="C66" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D66" s="42" t="str">
+      <c r="D66" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E66" s="42">
+      <c r="E66" s="37">
         <v>0</v>
       </c>
-      <c r="F66" s="41">
+      <c r="F66" s="36">
         <v>200</v>
       </c>
-      <c r="G66" s="43" t="s">
+      <c r="G66" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H66" s="41" t="s">
+      <c r="H66" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I66" s="41"/>
-      <c r="J66" s="41">
+      <c r="I66" s="36"/>
+      <c r="J66" s="36">
         <v>0</v>
       </c>
-      <c r="K66" s="41" t="s">
+      <c r="K66" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L66" s="41">
+      <c r="L66" s="36">
         <v>6</v>
       </c>
-      <c r="M66" s="41" t="s">
+      <c r="M66" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N66" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O66" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P66" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q66" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R66" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S66" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T66" s="45"/>
-    </row>
-    <row r="67" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="41">
+      <c r="N66" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O66" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P66" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q66" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R66" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S66" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T66" s="40"/>
+    </row>
+    <row r="67" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="36">
         <v>49</v>
       </c>
-      <c r="B67" s="41" t="s">
+      <c r="B67" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="C67" s="42" t="s">
+      <c r="C67" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D67" s="42" t="str">
+      <c r="D67" s="37" t="str">
         <f t="shared" ref="D67" si="12">LEFT(C67, FIND("-", C67)-1)</f>
         <v>numeric</v>
       </c>
-      <c r="E67" s="42">
+      <c r="E67" s="37">
         <v>0</v>
       </c>
-      <c r="F67" s="41">
+      <c r="F67" s="36">
         <v>1000</v>
       </c>
-      <c r="G67" s="43" t="s">
+      <c r="G67" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H67" s="41" t="s">
+      <c r="H67" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I67" s="41"/>
-      <c r="J67" s="41">
+      <c r="I67" s="36"/>
+      <c r="J67" s="36">
         <v>0</v>
       </c>
-      <c r="K67" s="41" t="s">
+      <c r="K67" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L67" s="41">
+      <c r="L67" s="36">
         <v>24</v>
       </c>
-      <c r="M67" s="41" t="s">
+      <c r="M67" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N67" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O67" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P67" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q67" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R67" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S67" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T67" s="45"/>
-    </row>
-    <row r="68" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="41">
+      <c r="N67" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O67" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P67" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q67" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R67" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S67" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T67" s="40"/>
+    </row>
+    <row r="68" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="36">
         <v>50</v>
       </c>
-      <c r="B68" s="41" t="s">
+      <c r="B68" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="C68" s="42" t="s">
+      <c r="C68" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D68" s="42" t="str">
+      <c r="D68" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E68" s="42">
+      <c r="E68" s="37">
         <v>0</v>
       </c>
-      <c r="F68" s="41">
+      <c r="F68" s="36">
         <v>10</v>
       </c>
-      <c r="G68" s="43" t="s">
+      <c r="G68" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H68" s="41" t="s">
+      <c r="H68" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I68" s="41"/>
-      <c r="J68" s="41">
+      <c r="I68" s="36"/>
+      <c r="J68" s="36">
         <v>0</v>
       </c>
-      <c r="K68" s="41" t="s">
+      <c r="K68" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L68" s="41">
+      <c r="L68" s="36">
         <v>6</v>
       </c>
-      <c r="M68" s="41" t="s">
+      <c r="M68" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N68" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O68" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P68" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q68" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R68" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S68" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T68" s="45"/>
-    </row>
-    <row r="69" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="41">
+      <c r="N68" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O68" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P68" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q68" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R68" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S68" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T68" s="40"/>
+    </row>
+    <row r="69" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="36">
         <v>51</v>
       </c>
-      <c r="B69" s="41" t="s">
+      <c r="B69" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="C69" s="42" t="s">
+      <c r="C69" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D69" s="42" t="str">
+      <c r="D69" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E69" s="42">
+      <c r="E69" s="37">
         <v>0</v>
       </c>
-      <c r="F69" s="41">
+      <c r="F69" s="36">
         <v>1000</v>
       </c>
-      <c r="G69" s="43" t="s">
+      <c r="G69" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H69" s="41" t="s">
+      <c r="H69" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I69" s="41"/>
-      <c r="J69" s="41">
+      <c r="I69" s="36"/>
+      <c r="J69" s="36">
         <v>0</v>
       </c>
-      <c r="K69" s="41" t="s">
+      <c r="K69" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L69" s="41">
+      <c r="L69" s="36">
         <v>24</v>
       </c>
-      <c r="M69" s="41" t="s">
+      <c r="M69" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N69" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O69" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P69" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q69" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R69" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S69" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T69" s="45"/>
-    </row>
-    <row r="70" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="41">
+      <c r="N69" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O69" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P69" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q69" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R69" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S69" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T69" s="40"/>
+    </row>
+    <row r="70" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="36">
         <v>52</v>
       </c>
-      <c r="B70" s="41" t="s">
+      <c r="B70" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="C70" s="42" t="s">
+      <c r="C70" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D70" s="42" t="str">
+      <c r="D70" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E70" s="42">
+      <c r="E70" s="37">
         <v>0</v>
       </c>
-      <c r="F70" s="41">
+      <c r="F70" s="36">
         <v>1000</v>
       </c>
-      <c r="G70" s="43" t="s">
+      <c r="G70" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H70" s="41" t="s">
+      <c r="H70" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I70" s="41"/>
-      <c r="J70" s="41">
+      <c r="I70" s="36"/>
+      <c r="J70" s="36">
         <v>0</v>
       </c>
-      <c r="K70" s="41" t="s">
+      <c r="K70" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L70" s="41">
+      <c r="L70" s="36">
         <v>24</v>
       </c>
-      <c r="M70" s="41" t="s">
+      <c r="M70" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N70" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O70" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P70" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q70" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R70" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S70" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T70" s="45"/>
-    </row>
-    <row r="71" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="41">
+      <c r="N70" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O70" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P70" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q70" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R70" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S70" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T70" s="40"/>
+    </row>
+    <row r="71" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="36">
         <v>53</v>
       </c>
-      <c r="B71" s="41" t="s">
+      <c r="B71" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="C71" s="42" t="s">
+      <c r="C71" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D71" s="42" t="str">
+      <c r="D71" s="37" t="str">
         <f t="shared" ref="D71" si="13">LEFT(C71, FIND("-", C71)-1)</f>
         <v>numeric</v>
       </c>
-      <c r="E71" s="42">
+      <c r="E71" s="37">
         <v>0</v>
       </c>
-      <c r="F71" s="41">
+      <c r="F71" s="36">
         <v>1000</v>
       </c>
-      <c r="G71" s="43" t="s">
+      <c r="G71" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H71" s="41" t="s">
+      <c r="H71" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I71" s="41"/>
-      <c r="J71" s="41">
+      <c r="I71" s="36"/>
+      <c r="J71" s="36">
         <v>0</v>
       </c>
-      <c r="K71" s="41" t="s">
+      <c r="K71" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L71" s="41">
+      <c r="L71" s="36">
         <v>24</v>
       </c>
-      <c r="M71" s="41" t="s">
+      <c r="M71" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N71" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O71" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P71" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q71" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R71" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S71" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T71" s="45"/>
-    </row>
-    <row r="72" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="41">
+      <c r="N71" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O71" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P71" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q71" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R71" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S71" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T71" s="40"/>
+    </row>
+    <row r="72" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="36">
         <v>54</v>
       </c>
-      <c r="B72" s="41" t="s">
+      <c r="B72" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="C72" s="42" t="s">
+      <c r="C72" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D72" s="42" t="str">
+      <c r="D72" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E72" s="42">
+      <c r="E72" s="37">
         <v>0</v>
       </c>
-      <c r="F72" s="41">
+      <c r="F72" s="36">
         <v>10</v>
       </c>
-      <c r="G72" s="43" t="s">
+      <c r="G72" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H72" s="41" t="s">
+      <c r="H72" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I72" s="41"/>
-      <c r="J72" s="41">
+      <c r="I72" s="36"/>
+      <c r="J72" s="36">
         <v>0</v>
       </c>
-      <c r="K72" s="41" t="s">
+      <c r="K72" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L72" s="41">
+      <c r="L72" s="36">
         <v>12</v>
       </c>
-      <c r="M72" s="41" t="s">
+      <c r="M72" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N72" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O72" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P72" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q72" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R72" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S72" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T72" s="45"/>
-    </row>
-    <row r="73" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="41">
-        <v>55</v>
-      </c>
-      <c r="B73" s="41" t="s">
+      <c r="N72" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O72" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P72" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q72" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R72" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S72" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T72" s="40"/>
+    </row>
+    <row r="73" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="36">
+        <v>55</v>
+      </c>
+      <c r="B73" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="C73" s="42" t="s">
+      <c r="C73" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D73" s="42" t="str">
+      <c r="D73" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E73" s="42">
+      <c r="E73" s="37">
         <v>0</v>
       </c>
-      <c r="F73" s="41">
+      <c r="F73" s="36">
         <v>50</v>
       </c>
-      <c r="G73" s="43" t="s">
+      <c r="G73" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H73" s="41" t="s">
+      <c r="H73" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I73" s="41"/>
-      <c r="J73" s="41">
+      <c r="I73" s="36"/>
+      <c r="J73" s="36">
         <v>0</v>
       </c>
-      <c r="K73" s="41" t="s">
+      <c r="K73" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L73" s="41">
+      <c r="L73" s="36">
         <v>6</v>
       </c>
-      <c r="M73" s="41" t="s">
+      <c r="M73" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N73" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O73" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P73" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q73" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R73" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S73" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T73" s="45"/>
-    </row>
-    <row r="74" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="41">
+      <c r="N73" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O73" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P73" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q73" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R73" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S73" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T73" s="40"/>
+    </row>
+    <row r="74" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="36">
         <v>56</v>
       </c>
-      <c r="B74" s="41" t="s">
+      <c r="B74" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="C74" s="42" t="s">
+      <c r="C74" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D74" s="42" t="str">
+      <c r="D74" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E74" s="42">
+      <c r="E74" s="37">
         <v>0</v>
       </c>
-      <c r="F74" s="41">
+      <c r="F74" s="36">
         <v>100</v>
       </c>
-      <c r="G74" s="43" t="s">
+      <c r="G74" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H74" s="41" t="s">
+      <c r="H74" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I74" s="41"/>
-      <c r="J74" s="41">
+      <c r="I74" s="36"/>
+      <c r="J74" s="36">
         <v>0</v>
       </c>
-      <c r="K74" s="41" t="s">
+      <c r="K74" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L74" s="41">
+      <c r="L74" s="36">
         <v>4</v>
       </c>
-      <c r="M74" s="41" t="s">
+      <c r="M74" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="N74" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O74" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P74" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q74" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R74" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S74" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T74" s="45"/>
-    </row>
-    <row r="75" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="41">
+      <c r="N74" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O74" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P74" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q74" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R74" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S74" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T74" s="40"/>
+    </row>
+    <row r="75" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="36">
         <v>57</v>
       </c>
-      <c r="B75" s="41" t="s">
+      <c r="B75" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="C75" s="42" t="s">
+      <c r="C75" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D75" s="42" t="str">
+      <c r="D75" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E75" s="42">
+      <c r="E75" s="37">
         <v>0</v>
       </c>
-      <c r="F75" s="41">
+      <c r="F75" s="36">
         <v>1000</v>
       </c>
-      <c r="G75" s="43" t="s">
+      <c r="G75" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H75" s="41" t="s">
+      <c r="H75" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I75" s="41"/>
-      <c r="J75" s="41">
+      <c r="I75" s="36"/>
+      <c r="J75" s="36">
         <v>0</v>
       </c>
-      <c r="K75" s="41" t="s">
+      <c r="K75" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L75" s="41">
+      <c r="L75" s="36">
         <v>2</v>
       </c>
-      <c r="M75" s="41" t="s">
+      <c r="M75" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="N75" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O75" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P75" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q75" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R75" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S75" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T75" s="45"/>
-    </row>
-    <row r="76" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="41">
+      <c r="N75" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O75" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P75" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q75" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R75" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S75" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T75" s="40"/>
+    </row>
+    <row r="76" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="36">
         <v>58</v>
       </c>
-      <c r="B76" s="41" t="s">
+      <c r="B76" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="C76" s="42" t="s">
+      <c r="C76" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D76" s="42" t="str">
+      <c r="D76" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E76" s="42">
+      <c r="E76" s="37">
         <v>0</v>
       </c>
-      <c r="F76" s="41">
+      <c r="F76" s="36">
         <v>300</v>
       </c>
-      <c r="G76" s="43" t="s">
+      <c r="G76" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H76" s="41" t="s">
+      <c r="H76" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I76" s="41"/>
-      <c r="J76" s="41">
+      <c r="I76" s="36"/>
+      <c r="J76" s="36">
         <v>0</v>
       </c>
-      <c r="K76" s="41" t="s">
+      <c r="K76" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L76" s="41">
+      <c r="L76" s="36">
         <v>1</v>
       </c>
-      <c r="M76" s="41" t="s">
+      <c r="M76" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N76" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O76" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P76" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q76" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R76" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S76" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T76" s="45"/>
-    </row>
-    <row r="77" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="41">
+      <c r="N76" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O76" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P76" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q76" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R76" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S76" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T76" s="40"/>
+    </row>
+    <row r="77" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="36">
         <v>59</v>
       </c>
-      <c r="B77" s="41" t="s">
+      <c r="B77" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="C77" s="42" t="s">
+      <c r="C77" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D77" s="42" t="str">
+      <c r="D77" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E77" s="42">
+      <c r="E77" s="37">
         <v>0</v>
       </c>
-      <c r="F77" s="41">
+      <c r="F77" s="36">
         <v>300</v>
       </c>
-      <c r="G77" s="43" t="s">
+      <c r="G77" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H77" s="41" t="s">
+      <c r="H77" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I77" s="41"/>
-      <c r="J77" s="41">
+      <c r="I77" s="36"/>
+      <c r="J77" s="36">
         <v>0</v>
       </c>
-      <c r="K77" s="41" t="s">
+      <c r="K77" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L77" s="41">
+      <c r="L77" s="36">
         <v>1</v>
       </c>
-      <c r="M77" s="41" t="s">
+      <c r="M77" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N77" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O77" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P77" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q77" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R77" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S77" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T77" s="45"/>
-    </row>
-    <row r="78" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="41">
+      <c r="N77" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O77" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P77" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q77" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R77" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S77" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T77" s="40"/>
+    </row>
+    <row r="78" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="36">
         <v>60</v>
       </c>
-      <c r="B78" s="41" t="s">
+      <c r="B78" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="C78" s="42" t="s">
+      <c r="C78" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="42" t="str">
+      <c r="D78" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E78" s="42">
+      <c r="E78" s="37">
         <v>0</v>
       </c>
-      <c r="F78" s="41">
+      <c r="F78" s="36">
         <v>200</v>
       </c>
-      <c r="G78" s="43" t="s">
+      <c r="G78" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H78" s="41" t="s">
+      <c r="H78" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I78" s="41"/>
-      <c r="J78" s="41">
+      <c r="I78" s="36"/>
+      <c r="J78" s="36">
         <v>0</v>
       </c>
-      <c r="K78" s="41" t="s">
+      <c r="K78" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L78" s="41">
+      <c r="L78" s="36">
         <v>1</v>
       </c>
-      <c r="M78" s="41" t="s">
+      <c r="M78" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N78" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O78" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P78" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q78" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R78" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S78" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T78" s="45"/>
-    </row>
-    <row r="79" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="41">
+      <c r="N78" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O78" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P78" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q78" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R78" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S78" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T78" s="40"/>
+    </row>
+    <row r="79" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="36">
         <v>61</v>
       </c>
-      <c r="B79" s="41" t="s">
+      <c r="B79" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="C79" s="42" t="s">
+      <c r="C79" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D79" s="42" t="str">
+      <c r="D79" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E79" s="42">
+      <c r="E79" s="37">
         <v>0</v>
       </c>
-      <c r="F79" s="41">
+      <c r="F79" s="36">
         <v>250</v>
       </c>
-      <c r="G79" s="43" t="s">
+      <c r="G79" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H79" s="41" t="s">
+      <c r="H79" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I79" s="41"/>
-      <c r="J79" s="41">
+      <c r="I79" s="36"/>
+      <c r="J79" s="36">
         <v>0</v>
       </c>
-      <c r="K79" s="41" t="s">
+      <c r="K79" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L79" s="41">
+      <c r="L79" s="36">
         <v>1</v>
       </c>
-      <c r="M79" s="41" t="s">
+      <c r="M79" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N79" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O79" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P79" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q79" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R79" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S79" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T79" s="45"/>
-    </row>
-    <row r="80" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="41">
+      <c r="N79" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O79" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P79" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q79" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R79" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S79" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T79" s="40"/>
+    </row>
+    <row r="80" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="36">
         <v>62</v>
       </c>
-      <c r="B80" s="41" t="s">
+      <c r="B80" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="C80" s="42" t="s">
+      <c r="C80" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D80" s="42" t="str">
+      <c r="D80" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E80" s="42">
+      <c r="E80" s="37">
         <v>0</v>
       </c>
-      <c r="F80" s="41">
+      <c r="F80" s="36">
         <v>200</v>
       </c>
-      <c r="G80" s="43" t="s">
+      <c r="G80" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H80" s="41" t="s">
+      <c r="H80" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I80" s="41"/>
-      <c r="J80" s="41">
+      <c r="I80" s="36"/>
+      <c r="J80" s="36">
         <v>0</v>
       </c>
-      <c r="K80" s="41" t="s">
+      <c r="K80" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L80" s="41">
+      <c r="L80" s="36">
         <v>1</v>
       </c>
-      <c r="M80" s="41" t="s">
+      <c r="M80" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="N80" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O80" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P80" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q80" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R80" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S80" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T80" s="45"/>
-    </row>
-    <row r="81" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="41">
+      <c r="N80" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O80" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P80" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q80" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R80" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S80" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T80" s="40"/>
+    </row>
+    <row r="81" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="36">
         <v>63</v>
       </c>
-      <c r="B81" s="41" t="s">
+      <c r="B81" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="C81" s="42" t="s">
+      <c r="C81" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D81" s="42" t="str">
+      <c r="D81" s="37" t="str">
         <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
-      <c r="E81" s="42">
+      <c r="E81" s="37">
         <v>0</v>
       </c>
-      <c r="F81" s="41">
+      <c r="F81" s="36">
         <v>100</v>
       </c>
-      <c r="G81" s="43" t="s">
+      <c r="G81" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H81" s="41" t="s">
+      <c r="H81" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I81" s="41"/>
-      <c r="J81" s="41">
+      <c r="I81" s="36"/>
+      <c r="J81" s="36">
         <v>0</v>
       </c>
-      <c r="K81" s="41" t="s">
+      <c r="K81" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L81" s="41">
+      <c r="L81" s="36">
         <v>14</v>
       </c>
-      <c r="M81" s="41" t="s">
+      <c r="M81" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="N81" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O81" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P81" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q81" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R81" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S81" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="T81" s="45"/>
+      <c r="N81" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O81" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P81" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q81" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R81" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S81" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="T81" s="40"/>
     </row>
     <row r="82" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="41">
+      <c r="A82" s="36">
         <v>64</v>
       </c>
-      <c r="B82" s="41" t="s">
+      <c r="B82" s="36" t="s">
         <v>249</v>
       </c>
-      <c r="C82" s="42" t="s">
+      <c r="C82" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D82" s="42" t="str">
+      <c r="D82" s="37" t="str">
         <f t="shared" ref="D82:D83" si="14">LEFT(C82, FIND("-", C82)-1)</f>
         <v>numeric</v>
       </c>
-      <c r="E82" s="42">
+      <c r="E82" s="37">
         <v>0</v>
       </c>
-      <c r="F82" s="41">
+      <c r="F82" s="36">
         <v>1000000</v>
       </c>
-      <c r="G82" s="43" t="s">
+      <c r="G82" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H82" s="41" t="s">
+      <c r="H82" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I82" s="41"/>
-      <c r="J82" s="41">
+      <c r="I82" s="36"/>
+      <c r="J82" s="36">
         <v>0</v>
       </c>
-      <c r="K82" s="41" t="s">
+      <c r="K82" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L82" s="41">
+      <c r="L82" s="36">
         <v>24</v>
       </c>
-      <c r="M82" s="41" t="s">
+      <c r="M82" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N82" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O82" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P82" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q82" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R82" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S82" s="44" t="s">
+      <c r="N82" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O82" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P82" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q82" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R82" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S82" s="39" t="s">
         <v>55</v>
       </c>
       <c r="T82" s="4"/>
     </row>
     <row r="83" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="41">
+      <c r="A83" s="36">
         <v>65</v>
       </c>
-      <c r="B83" s="41" t="s">
+      <c r="B83" s="36" t="s">
         <v>250</v>
       </c>
-      <c r="C83" s="42" t="s">
+      <c r="C83" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D83" s="42" t="str">
+      <c r="D83" s="37" t="str">
         <f t="shared" si="14"/>
         <v>numeric</v>
       </c>
-      <c r="E83" s="42">
+      <c r="E83" s="37">
         <v>0</v>
       </c>
-      <c r="F83" s="41">
+      <c r="F83" s="36">
         <v>1000</v>
       </c>
-      <c r="G83" s="43" t="s">
+      <c r="G83" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H83" s="41" t="s">
+      <c r="H83" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I83" s="41"/>
-      <c r="J83" s="41">
+      <c r="I83" s="36"/>
+      <c r="J83" s="36">
         <v>0</v>
       </c>
-      <c r="K83" s="41" t="s">
+      <c r="K83" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L83" s="41">
+      <c r="L83" s="36">
         <v>1</v>
       </c>
-      <c r="M83" s="41" t="s">
+      <c r="M83" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="N83" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O83" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P83" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q83" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R83" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S83" s="44" t="s">
+      <c r="N83" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O83" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P83" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q83" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R83" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S83" s="39" t="s">
         <v>55</v>
       </c>
       <c r="T83" s="4"/>
     </row>
     <row r="84" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="41">
+      <c r="A84" s="36">
         <v>66</v>
       </c>
-      <c r="B84" s="41" t="s">
+      <c r="B84" s="36" t="s">
         <v>251</v>
       </c>
-      <c r="C84" s="42" t="s">
+      <c r="C84" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="42" t="str">
+      <c r="D84" s="37" t="str">
         <f t="shared" ref="D84:D85" si="15">LEFT(C84, FIND("-", C84)-1)</f>
         <v>numeric</v>
       </c>
-      <c r="E84" s="42">
+      <c r="E84" s="37">
         <v>0</v>
       </c>
-      <c r="F84" s="41">
+      <c r="F84" s="36">
         <v>100</v>
       </c>
-      <c r="G84" s="43" t="s">
+      <c r="G84" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H84" s="41" t="s">
+      <c r="H84" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I84" s="41"/>
-      <c r="J84" s="41">
+      <c r="I84" s="36"/>
+      <c r="J84" s="36">
         <v>0</v>
       </c>
-      <c r="K84" s="41" t="s">
+      <c r="K84" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L84" s="41">
+      <c r="L84" s="36">
         <v>6</v>
       </c>
-      <c r="M84" s="41" t="s">
+      <c r="M84" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N84" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O84" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P84" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q84" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R84" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S84" s="44" t="s">
+      <c r="N84" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O84" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P84" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q84" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R84" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S84" s="39" t="s">
         <v>55</v>
       </c>
       <c r="T84" s="4"/>
     </row>
     <row r="85" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="41">
+      <c r="A85" s="36">
         <v>67</v>
       </c>
-      <c r="B85" s="41" t="s">
+      <c r="B85" s="36" t="s">
         <v>252</v>
       </c>
-      <c r="C85" s="42" t="s">
+      <c r="C85" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D85" s="42" t="str">
+      <c r="D85" s="37" t="str">
         <f t="shared" si="15"/>
         <v>numeric</v>
       </c>
-      <c r="E85" s="42">
+      <c r="E85" s="37">
         <v>0</v>
       </c>
-      <c r="F85" s="41">
+      <c r="F85" s="36">
         <v>100</v>
       </c>
-      <c r="G85" s="43" t="s">
+      <c r="G85" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H85" s="41" t="s">
+      <c r="H85" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="I85" s="41"/>
-      <c r="J85" s="41">
+      <c r="I85" s="36"/>
+      <c r="J85" s="36">
         <v>0</v>
       </c>
-      <c r="K85" s="41" t="s">
+      <c r="K85" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="L85" s="41">
+      <c r="L85" s="36">
         <v>6</v>
       </c>
-      <c r="M85" s="41" t="s">
+      <c r="M85" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="N85" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="O85" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P85" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q85" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="R85" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="S85" s="44" t="s">
+      <c r="N85" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O85" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P85" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q85" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R85" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="S85" s="39" t="s">
         <v>55</v>
       </c>
       <c r="T85" s="4"/>
@@ -24386,9 +24376,9 @@
   </sheetPr>
   <dimension ref="A1:AF994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -25072,7 +25062,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <f t="shared" ref="A13:A43" si="1">1000+C13</f>
+        <f t="shared" ref="A13:A46" si="1">1000+C13</f>
         <v>1036</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -26545,7 +26535,7 @@
       <c r="E40" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F40" s="48" t="s">
+      <c r="F40" s="43" t="s">
         <v>253</v>
       </c>
       <c r="G40" s="5" t="s">
@@ -26745,61 +26735,160 @@
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+      <c r="A44" s="3">
+        <f t="shared" si="1"/>
+        <v>1071</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C44" s="3">
+        <v>71</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
+      <c r="G44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J44" s="3">
+        <v>12</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L44" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="O44" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="P44" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q44" s="12" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
+      <c r="A45" s="3">
+        <f t="shared" si="1"/>
+        <v>1081</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C45" s="3">
+        <v>81</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="15"/>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="15"/>
+      <c r="G45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J45" s="3">
+        <v>12</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L45" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M45" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N45" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="O45" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="P45" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q45" s="12" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+      <c r="A46" s="3">
+        <f t="shared" si="1"/>
+        <v>1082</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C46" s="3">
+        <v>82</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="15"/>
-      <c r="P46" s="15"/>
-      <c r="Q46" s="15"/>
+      <c r="G46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H46" s="3">
+        <v>0</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J46" s="3">
+        <v>12</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L46" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M46" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N46" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="O46" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="P46" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q46" s="12" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
@@ -44821,7 +44910,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{25F64F70-E844-451E-A092-027E82FEE113}">
       <formula1>"min, max"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576 I2:I1048576" xr:uid="{05752E7E-6681-422B-A153-73C89C26B8FC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576 K2:K1048576" xr:uid="{05752E7E-6681-422B-A153-73C89C26B8FC}">
       <formula1>"second, minute, hour, day, week, month, year"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C40:C43 A2:A1048576" xr:uid="{B0B8DD5B-800F-4696-AA1D-3B2D767EBEBC}">
@@ -44845,8 +44934,8 @@
   <dimension ref="A1:X1017"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -58856,13 +58945,13 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" style="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.88671875" style="23" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
adding functionality to build trends
</commit_message>
<xml_diff>
--- a/taks.xlsx
+++ b/taks.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonat\CodeProjects\TAKAutomator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC525DF5-4E37-46D2-8E1A-1E821C7AD4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15E571F-03A0-41CB-8971-878BF50C7AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_concepts" sheetId="1" r:id="rId1"/>
     <sheet name="states" sheetId="2" r:id="rId2"/>
     <sheet name="events" sheetId="3" r:id="rId3"/>
     <sheet name="contexts" sheetId="5" r:id="rId4"/>
-    <sheet name="patterns" sheetId="4" r:id="rId5"/>
-    <sheet name="scenarios" sheetId="6" r:id="rId6"/>
+    <sheet name="trends" sheetId="7" r:id="rId5"/>
+    <sheet name="patterns" sheetId="4" r:id="rId6"/>
+    <sheet name="scenarios" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">raw_concepts!$A$1:$T$907</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="351">
   <si>
     <t>TYPE</t>
   </si>
@@ -963,6 +964,141 @@
   <si>
     <t>INFECTION_EVENT</t>
   </si>
+  <si>
+    <t>SIGNIFICANT_VARIATION</t>
+  </si>
+  <si>
+    <t>TIME_STEADY_VALUE</t>
+  </si>
+  <si>
+    <t>TIME_STEADY_UNIT</t>
+  </si>
+  <si>
+    <t>GLUCOSE_LEVEL_EVENT</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>Measurements</t>
+  </si>
+  <si>
+    <t>GLUCOSE_MEASURE_LAB_TREND</t>
+  </si>
+  <si>
+    <t>GLUCOSE_MEASURE_CAPILLARY_TREND</t>
+  </si>
+  <si>
+    <t>HEMOGLOBIN_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>HEMOGLOBIN_DISTRIBUTION_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>HEMOGLOBIN-A1C_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>HEMATOCRIT_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>MCV_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>MCH_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>LYMPHOCYTES_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>NEUTROPHILS_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>MONOCYTES_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>RDW_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>PLT_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>PLT_DISTRIBUTION_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>MPV_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>CREATININE_MEASURE_SERUM_TREND</t>
+  </si>
+  <si>
+    <t>CREATININE_MEASURE_URINE_TREND</t>
+  </si>
+  <si>
+    <t>UREA_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>ALBUMIN_MEASURE_SERUM_TREND</t>
+  </si>
+  <si>
+    <t>ALBUMIN_MEASURE_URINE_TREND</t>
+  </si>
+  <si>
+    <t>SODIUM_MEASURE_BLOOD_TREND</t>
+  </si>
+  <si>
+    <t>SODIUM_MEASURE_URINE_TREND</t>
+  </si>
+  <si>
+    <t>POTASSIUM_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>ASPARATE-AMINOTRANSFERASE_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>ALANINE-AMINOTRANSFERASE_SERUM_TREND</t>
+  </si>
+  <si>
+    <t>ALANINE-AMINOTRANSFERASE_BLOOD_TREND</t>
+  </si>
+  <si>
+    <t>PH_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>BICARBONATE_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>ALKALINE-PHOSPHATASE_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>BLOOD_PRESSURE_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>BLOOD_PRESSURE_SYSTOLIC_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>BLOOD_PRESSURE_DIASTOLIC_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>HEART_RATE_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>E-GFR_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>CREATINE-KINASE_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>CHOLESTEROL_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>TROPONIN_SERUM_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>TROPONIN_BLOOD_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>GLUCOSE_LEVEL_TREND</t>
+  </si>
 </sst>
 </file>
 
@@ -1046,7 +1182,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1095,11 +1231,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1214,6 +1365,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1435,8 +1599,8 @@
   <dimension ref="A1:T907"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24305,9 +24469,9 @@
   </sheetPr>
   <dimension ref="A1:AF993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -44806,11 +44970,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X1017"/>
+  <dimension ref="A1:X1018"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -44825,7 +44989,7 @@
     <col min="8" max="8" width="15.44140625" style="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.109375" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.21875" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -44876,116 +45040,115 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:24" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45">
         <v>1104</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="45" t="s">
         <v>289</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="E2" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="45"/>
+    </row>
+    <row r="3" spans="1:24" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45">
         <v>1105</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="45" t="s">
         <v>290</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <f>1100+C4</f>
-        <v>1170</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="C4" s="3">
-        <v>70</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="3"/>
+      <c r="E3" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" s="45"/>
+    </row>
+    <row r="4" spans="1:24" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45">
+        <v>1101</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>310</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>311</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="45"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <f t="shared" ref="A5:A35" si="0">1100+C5</f>
-        <v>1172</v>
+        <f>1100+C5</f>
+        <v>1170</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C5" s="3">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>235</v>
@@ -45012,14 +45175,14 @@
     </row>
     <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <f t="shared" si="0"/>
-        <v>1173</v>
+        <f t="shared" ref="A6:A36" si="0">1100+C6</f>
+        <v>1172</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C6" s="3">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>235</v>
@@ -45047,13 +45210,13 @@
     <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C7" s="3">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>235</v>
@@ -45081,13 +45244,13 @@
     <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C8" s="3">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>235</v>
@@ -45115,13 +45278,13 @@
     <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="C9" s="3">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>235</v>
@@ -45149,13 +45312,13 @@
     <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="C10" s="3">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>235</v>
@@ -45183,13 +45346,13 @@
     <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C11" s="3">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>235</v>
@@ -45217,13 +45380,13 @@
     <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C12" s="3">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>235</v>
@@ -45251,13 +45414,13 @@
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="C13" s="3">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>235</v>
@@ -45285,13 +45448,13 @@
     <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
-        <v>1183</v>
+        <v>1180</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>258</v>
+        <v>288</v>
       </c>
       <c r="C14" s="3">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>235</v>
@@ -45319,13 +45482,13 @@
     <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C15" s="3">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>235</v>
@@ -45353,13 +45516,13 @@
     <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C16" s="3">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>235</v>
@@ -45387,13 +45550,13 @@
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C17" s="3">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>235</v>
@@ -45421,13 +45584,13 @@
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C18" s="3">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>235</v>
@@ -45455,16 +45618,16 @@
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
-        <v>1111</v>
+        <v>1187</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C19" s="3">
-        <v>11</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>112</v>
+        <v>87</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>235</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>55</v>
@@ -45479,7 +45642,7 @@
         <v>55</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J19" s="14" t="s">
         <v>55</v>
@@ -45489,16 +45652,16 @@
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C20" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>55</v>
@@ -45523,16 +45686,16 @@
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
-        <v>1110</v>
+        <v>1112</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C21" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>55</v>
@@ -45557,16 +45720,16 @@
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <f t="shared" si="0"/>
-        <v>1108</v>
+        <v>1110</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C22" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>55</v>
@@ -45591,13 +45754,13 @@
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <f t="shared" si="0"/>
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C23" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>115</v>
@@ -45625,13 +45788,13 @@
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <f t="shared" si="0"/>
-        <v>1113</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>268</v>
+        <v>1109</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="C24" s="3">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>115</v>
@@ -45659,13 +45822,13 @@
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <f t="shared" si="0"/>
-        <v>1114</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>269</v>
+        <v>1113</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>268</v>
       </c>
       <c r="C25" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>115</v>
@@ -45693,13 +45856,13 @@
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C26" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>115</v>
@@ -45727,13 +45890,13 @@
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C27" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>115</v>
@@ -45761,13 +45924,13 @@
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <f t="shared" si="0"/>
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C28" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>115</v>
@@ -45795,13 +45958,13 @@
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C29" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>115</v>
@@ -45829,13 +45992,13 @@
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C30" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>115</v>
@@ -45863,13 +46026,13 @@
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C31" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>115</v>
@@ -45897,13 +46060,13 @@
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <f t="shared" si="0"/>
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C32" s="3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>115</v>
@@ -45931,13 +46094,13 @@
     <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <f t="shared" si="0"/>
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>305</v>
+        <v>276</v>
       </c>
       <c r="C33" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>115</v>
@@ -45965,13 +46128,13 @@
     <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <f t="shared" si="0"/>
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>277</v>
+        <v>305</v>
       </c>
       <c r="C34" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>115</v>
@@ -45999,13 +46162,13 @@
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <f t="shared" si="0"/>
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C35" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>115</v>
@@ -46031,16 +46194,37 @@
       <c r="K35" s="3"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
+      <c r="A36" s="3">
+        <f t="shared" si="0"/>
+        <v>1124</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C36" s="3">
+        <v>24</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>55</v>
+      </c>
       <c r="K36" s="3"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -58796,12 +58980,25 @@
       <c r="J1017" s="14"/>
       <c r="K1017" s="3"/>
     </row>
+    <row r="1018" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1018" s="3"/>
+      <c r="B1018" s="3"/>
+      <c r="C1018" s="3"/>
+      <c r="D1018" s="3"/>
+      <c r="E1018" s="14"/>
+      <c r="F1018" s="14"/>
+      <c r="G1018" s="14"/>
+      <c r="H1018" s="14"/>
+      <c r="I1018" s="14"/>
+      <c r="J1018" s="14"/>
+      <c r="K1018" s="3"/>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576 C14:C35" xr:uid="{98A4E0C0-623A-43B0-A1B2-0ACD9C28F3FC}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576 C15:C36" xr:uid="{98A4E0C0-623A-43B0-A1B2-0ACD9C28F3FC}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Error" error="Currently, The implementation requires a derived from concept id, but the program is not planned to deal with TAKs that have more then 1 base concepts. Please focus on one at the time, or contact developers." sqref="C4:C13" xr:uid="{60DADC71-9D75-41E9-8E91-4A0A84ACE9E1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Error" error="Currently, The implementation requires a derived from concept id, but the program is not planned to deal with TAKs that have more then 1 base concepts. Please focus on one at the time, or contact developers." sqref="C5:C14" xr:uid="{60DADC71-9D75-41E9-8E91-4A0A84ACE9E1}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:J1048576" xr:uid="{BD14D827-2ED4-418B-B045-D2154EB50A63}">
       <formula1>"true, false"</formula1>
     </dataValidation>
@@ -58820,7 +59017,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -60179,6 +60376,885 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A161545-DA5F-4FD2-8279-D89A8EE73974}">
+  <dimension ref="A1:F40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" customWidth="1"/>
+    <col min="2" max="2" width="47.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>307</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <f t="shared" ref="A2" si="0">C2+1300</f>
+        <v>2401</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1101</v>
+      </c>
+      <c r="D2" s="23">
+        <v>30</v>
+      </c>
+      <c r="E2" s="23">
+        <v>24</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <f>C3+1300</f>
+        <v>1301</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="23">
+        <v>40</v>
+      </c>
+      <c r="E3" s="23">
+        <v>24</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A40" si="1">C4+1300</f>
+        <v>1302</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="23">
+        <v>30</v>
+      </c>
+      <c r="E4" s="23">
+        <v>24</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <f t="shared" si="1"/>
+        <v>1330</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C5" s="3">
+        <v>30</v>
+      </c>
+      <c r="D5" s="23">
+        <v>5</v>
+      </c>
+      <c r="E5" s="23">
+        <v>24</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <f t="shared" si="1"/>
+        <v>1331</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C6" s="3">
+        <v>31</v>
+      </c>
+      <c r="D6" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="E6" s="23">
+        <v>24</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <f t="shared" si="1"/>
+        <v>1332</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" s="3">
+        <v>32</v>
+      </c>
+      <c r="D7" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="23">
+        <v>24</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <f t="shared" si="1"/>
+        <v>1333</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C8" s="3">
+        <v>33</v>
+      </c>
+      <c r="D8" s="23">
+        <v>5</v>
+      </c>
+      <c r="E8" s="23">
+        <v>24</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <f t="shared" si="1"/>
+        <v>1334</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" s="3">
+        <v>34</v>
+      </c>
+      <c r="D9" s="23">
+        <v>10</v>
+      </c>
+      <c r="E9" s="23">
+        <v>24</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <f t="shared" si="1"/>
+        <v>1335</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C10" s="3">
+        <v>35</v>
+      </c>
+      <c r="D10" s="23">
+        <v>5</v>
+      </c>
+      <c r="E10" s="23">
+        <v>24</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <f t="shared" si="1"/>
+        <v>1336</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C11" s="3">
+        <v>36</v>
+      </c>
+      <c r="D11" s="23">
+        <v>5</v>
+      </c>
+      <c r="E11" s="23">
+        <v>24</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <f t="shared" si="1"/>
+        <v>1337</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C12" s="3">
+        <v>37</v>
+      </c>
+      <c r="D12" s="23">
+        <v>5</v>
+      </c>
+      <c r="E12" s="23">
+        <v>24</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <f t="shared" si="1"/>
+        <v>1338</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C13" s="3">
+        <v>38</v>
+      </c>
+      <c r="D13" s="23">
+        <v>5</v>
+      </c>
+      <c r="E13" s="23">
+        <v>24</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <f t="shared" si="1"/>
+        <v>1339</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C14" s="3">
+        <v>39</v>
+      </c>
+      <c r="D14" s="23">
+        <v>5</v>
+      </c>
+      <c r="E14" s="23">
+        <v>24</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <f t="shared" si="1"/>
+        <v>1340</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C15" s="3">
+        <v>40</v>
+      </c>
+      <c r="D15" s="23">
+        <v>50</v>
+      </c>
+      <c r="E15" s="23">
+        <v>24</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <f t="shared" si="1"/>
+        <v>1341</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C16" s="3">
+        <v>41</v>
+      </c>
+      <c r="D16" s="23">
+        <v>5</v>
+      </c>
+      <c r="E16" s="23">
+        <v>24</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <f t="shared" si="1"/>
+        <v>1342</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C17" s="3">
+        <v>42</v>
+      </c>
+      <c r="D17" s="23">
+        <v>5</v>
+      </c>
+      <c r="E17" s="23">
+        <v>24</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <f t="shared" si="1"/>
+        <v>1343</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C18" s="3">
+        <v>43</v>
+      </c>
+      <c r="D18" s="23">
+        <v>5</v>
+      </c>
+      <c r="E18" s="23">
+        <v>24</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <f t="shared" si="1"/>
+        <v>1344</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C19" s="3">
+        <v>44</v>
+      </c>
+      <c r="D19" s="23">
+        <v>2500</v>
+      </c>
+      <c r="E19" s="23">
+        <v>24</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <f t="shared" si="1"/>
+        <v>1345</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45</v>
+      </c>
+      <c r="D20" s="23">
+        <v>10</v>
+      </c>
+      <c r="E20" s="23">
+        <v>24</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <f t="shared" si="1"/>
+        <v>1346</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C21" s="3">
+        <v>46</v>
+      </c>
+      <c r="D21" s="23">
+        <v>5</v>
+      </c>
+      <c r="E21" s="23">
+        <v>24</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <f t="shared" si="1"/>
+        <v>1347</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C22" s="3">
+        <v>47</v>
+      </c>
+      <c r="D22" s="23">
+        <v>500</v>
+      </c>
+      <c r="E22" s="23">
+        <v>24</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <f t="shared" si="1"/>
+        <v>1348</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C23" s="3">
+        <v>48</v>
+      </c>
+      <c r="D23" s="23">
+        <v>10</v>
+      </c>
+      <c r="E23" s="23">
+        <v>24</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <f t="shared" si="1"/>
+        <v>1349</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C24" s="3">
+        <v>49</v>
+      </c>
+      <c r="D24" s="23">
+        <v>50</v>
+      </c>
+      <c r="E24" s="23">
+        <v>24</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <f t="shared" si="1"/>
+        <v>1350</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C25" s="3">
+        <v>50</v>
+      </c>
+      <c r="D25" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="23">
+        <v>24</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <f t="shared" si="1"/>
+        <v>1351</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C26" s="3">
+        <v>51</v>
+      </c>
+      <c r="D26" s="23">
+        <v>50</v>
+      </c>
+      <c r="E26" s="23">
+        <v>24</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <f t="shared" si="1"/>
+        <v>1352</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C27" s="3">
+        <v>52</v>
+      </c>
+      <c r="D27" s="23">
+        <v>50</v>
+      </c>
+      <c r="E27" s="23">
+        <v>24</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <f t="shared" si="1"/>
+        <v>1353</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C28" s="3">
+        <v>53</v>
+      </c>
+      <c r="D28" s="23">
+        <v>50</v>
+      </c>
+      <c r="E28" s="23">
+        <v>24</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <f t="shared" si="1"/>
+        <v>1354</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C29" s="3">
+        <v>54</v>
+      </c>
+      <c r="D29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="23">
+        <v>24</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <f t="shared" si="1"/>
+        <v>1355</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C30" s="3">
+        <v>55</v>
+      </c>
+      <c r="D30" s="23">
+        <v>2.5</v>
+      </c>
+      <c r="E30" s="23">
+        <v>24</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <f t="shared" si="1"/>
+        <v>1357</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C31" s="3">
+        <v>57</v>
+      </c>
+      <c r="D31" s="23">
+        <v>50</v>
+      </c>
+      <c r="E31" s="23">
+        <v>24</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <f t="shared" si="1"/>
+        <v>1358</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C32" s="3">
+        <v>58</v>
+      </c>
+      <c r="D32" s="23">
+        <v>15</v>
+      </c>
+      <c r="E32" s="23">
+        <v>24</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <f t="shared" si="1"/>
+        <v>1359</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C33" s="3">
+        <v>59</v>
+      </c>
+      <c r="D33" s="23">
+        <v>15</v>
+      </c>
+      <c r="E33" s="23">
+        <v>24</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <f t="shared" si="1"/>
+        <v>1360</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C34" s="3">
+        <v>60</v>
+      </c>
+      <c r="D34" s="23">
+        <v>10</v>
+      </c>
+      <c r="E34" s="23">
+        <v>24</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <f t="shared" si="1"/>
+        <v>1361</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C35" s="3">
+        <v>61</v>
+      </c>
+      <c r="D35" s="23">
+        <v>12.5</v>
+      </c>
+      <c r="E35" s="23">
+        <v>24</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <f t="shared" si="1"/>
+        <v>1362</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C36" s="3">
+        <v>62</v>
+      </c>
+      <c r="D36" s="23">
+        <v>10</v>
+      </c>
+      <c r="E36" s="23">
+        <v>24</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <f t="shared" si="1"/>
+        <v>1364</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C37" s="3">
+        <v>64</v>
+      </c>
+      <c r="D37" s="23">
+        <v>50000</v>
+      </c>
+      <c r="E37" s="23">
+        <v>24</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <f t="shared" si="1"/>
+        <v>1365</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C38" s="3">
+        <v>65</v>
+      </c>
+      <c r="D38" s="23">
+        <v>50</v>
+      </c>
+      <c r="E38" s="23">
+        <v>24</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <f t="shared" si="1"/>
+        <v>1366</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C39" s="3">
+        <v>66</v>
+      </c>
+      <c r="D39" s="23">
+        <v>5</v>
+      </c>
+      <c r="E39" s="23">
+        <v>24</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <f t="shared" si="1"/>
+        <v>1367</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C40" s="3">
+        <v>67</v>
+      </c>
+      <c r="D40" s="23">
+        <v>5</v>
+      </c>
+      <c r="E40" s="23">
+        <v>24</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="5">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Error" error="Currently, The implementation requires a derived from concept id, but the program is not planned to deal with TAKs that have more then 1 base concepts. Please focus on one at the time, or contact developers." sqref="C41:C1048576" xr:uid="{8ABBC965-E4AD-41DF-BBA6-1A0764036D82}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C40 A2:A1048576" xr:uid="{8FB02B24-4335-4796-A419-BD1D41E71A06}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D1048576 D2" xr:uid="{541E5BD0-9031-4A98-945D-A434CC5DE9D9}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{5ABE6B5A-333F-461C-9785-CAB0E7903CEF}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{0A768F11-6EE3-4A52-85B7-9AABF30B7B8F}">
+      <formula1>"second, minute, hour, day, week, month, year"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -61226,7 +62302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
update tak table and repo
</commit_message>
<xml_diff>
--- a/taks.xlsx
+++ b/taks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonat\CodeProjects\TAKAutomator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDF793E-D52F-4593-9055-3063EAC4F6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C8A2D1-7F6A-4872-B127-C75DB0088B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_concepts" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="scenarios" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">raw_concepts!$A$1:$T$907</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">raw_concepts!$A$1:$T$909</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="352">
   <si>
     <t>TYPE</t>
   </si>
@@ -612,9 +612,6 @@
     <t>OTHER_COMPLICATION_EVENT</t>
   </si>
   <si>
-    <t>DEMENTIA_EVENT</t>
-  </si>
-  <si>
     <t>CARDIOVASCULAR_DISORDER_EVENT</t>
   </si>
   <si>
@@ -1078,6 +1075,21 @@
   </si>
   <si>
     <t>ALANINE-AMINOTRANSFERASE_BLOOD_MEASURE_TREND</t>
+  </si>
+  <si>
+    <t>DEMENTIA_CONTEXT</t>
+  </si>
+  <si>
+    <t>HYPERGLYCEMIA</t>
+  </si>
+  <si>
+    <t>HYPOGLYCEMIA_EVENT</t>
+  </si>
+  <si>
+    <t>HYPERGLYCEMIA_EVENT</t>
+  </si>
+  <si>
+    <t>HYPOGLYCEMIA</t>
   </si>
 </sst>
 </file>
@@ -1563,11 +1575,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T907"/>
+  <dimension ref="A1:T909"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1655,13 +1667,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="2" t="str">
-        <f t="shared" ref="D2:D48" si="0">LEFT(C2, FIND("-", C2)-1)</f>
+        <f t="shared" ref="D2:D50" si="0">LEFT(C2, FIND("-", C2)-1)</f>
         <v>numeric</v>
       </c>
       <c r="E2" s="2">
@@ -1769,7 +1781,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>28</v>
@@ -2201,7 +2213,7 @@
         <v>76</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>27</v>
@@ -3579,7 +3591,7 @@
         <v>22</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>27</v>
@@ -3734,123 +3746,123 @@
       <c r="T40" s="29"/>
     </row>
     <row r="41" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="30">
-        <v>3</v>
-      </c>
-      <c r="B41" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="31" t="s">
+      <c r="A41" s="25">
+        <v>88</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>351</v>
+      </c>
+      <c r="C41" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="31" t="str">
-        <f t="shared" ref="D41" si="9">LEFT(C41, FIND("-", C41)-1)</f>
+      <c r="D41" s="27" t="str">
+        <f t="shared" ref="D41:D42" si="9">LEFT(C41, FIND("-", C41)-1)</f>
         <v>nominal</v>
       </c>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="30" t="s">
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="J41" s="30">
+      <c r="J41" s="25">
         <v>0</v>
       </c>
-      <c r="K41" s="30" t="s">
+      <c r="K41" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="L41" s="30">
-        <v>6</v>
-      </c>
-      <c r="M41" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="N41" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="O41" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="P41" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q41" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="R41" s="32" t="s">
+      <c r="L41" s="25">
+        <v>0</v>
+      </c>
+      <c r="M41" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="N41" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="O41" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="P41" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q41" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="R41" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="S41" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="T41" s="33"/>
+      <c r="S41" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="T41" s="29"/>
     </row>
     <row r="42" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="30">
-        <v>25</v>
-      </c>
-      <c r="B42" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="31" t="s">
+      <c r="A42" s="25">
+        <v>89</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="C42" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="31" t="str">
-        <f>LEFT(C42, FIND("-", C42)-1)</f>
+      <c r="D42" s="27" t="str">
+        <f t="shared" si="9"/>
         <v>nominal</v>
       </c>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="30" t="s">
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="J42" s="30">
+      <c r="J42" s="25">
         <v>0</v>
       </c>
-      <c r="K42" s="30" t="s">
+      <c r="K42" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="L42" s="30">
-        <v>6</v>
-      </c>
-      <c r="M42" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="N42" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="O42" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="P42" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q42" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="R42" s="32" t="s">
+      <c r="L42" s="25">
+        <v>0</v>
+      </c>
+      <c r="M42" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="N42" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="O42" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="P42" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q42" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="R42" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="S42" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="T42" s="33"/>
+      <c r="S42" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="T42" s="29"/>
     </row>
     <row r="43" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
       <c r="C43" s="31" t="s">
         <v>27</v>
       </c>
       <c r="D43" s="31" t="str">
-        <f>LEFT(C43, FIND("-", C43)-1)</f>
+        <f t="shared" ref="D43" si="10">LEFT(C43, FIND("-", C43)-1)</f>
         <v>nominal</v>
       </c>
       <c r="E43" s="31"/>
@@ -3894,10 +3906,10 @@
     </row>
     <row r="44" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="30">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C44" s="31" t="s">
         <v>27</v>
@@ -3947,10 +3959,10 @@
     </row>
     <row r="45" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="30">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
       <c r="C45" s="31" t="s">
         <v>27</v>
@@ -3999,150 +4011,138 @@
       <c r="T45" s="33"/>
     </row>
     <row r="46" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="34">
+      <c r="A46" s="30">
+        <v>27</v>
+      </c>
+      <c r="B46" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" s="31" t="str">
+        <f>LEFT(C46, FIND("-", C46)-1)</f>
+        <v>nominal</v>
+      </c>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="31"/>
+      <c r="I46" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J46" s="30">
+        <v>0</v>
+      </c>
+      <c r="K46" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="L46" s="30">
+        <v>6</v>
+      </c>
+      <c r="M46" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="N46" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="O46" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="P46" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q46" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="R46" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="S46" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="T46" s="33"/>
+    </row>
+    <row r="47" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="30">
+        <v>28</v>
+      </c>
+      <c r="B47" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" s="31" t="str">
+        <f>LEFT(C47, FIND("-", C47)-1)</f>
+        <v>nominal</v>
+      </c>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J47" s="30">
+        <v>0</v>
+      </c>
+      <c r="K47" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="L47" s="30">
+        <v>6</v>
+      </c>
+      <c r="M47" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="N47" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="O47" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="P47" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q47" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="R47" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="S47" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="T47" s="33"/>
+    </row>
+    <row r="48" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="34">
         <v>1</v>
       </c>
-      <c r="B46" s="35" t="s">
-        <v>292</v>
-      </c>
-      <c r="C46" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="D46" s="35" t="str">
-        <f t="shared" ref="D46:D47" si="10">LEFT(C46, FIND("-", C46)-1)</f>
-        <v>numeric</v>
-      </c>
-      <c r="E46" s="35">
-        <v>0</v>
-      </c>
-      <c r="F46" s="36">
-        <v>800</v>
-      </c>
-      <c r="G46" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="H46" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="I46" s="35"/>
-      <c r="J46" s="34">
-        <v>0</v>
-      </c>
-      <c r="K46" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="L46" s="34">
-        <v>24</v>
-      </c>
-      <c r="M46" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="N46" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="O46" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="P46" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q46" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="R46" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="S46" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="T46" s="38"/>
-    </row>
-    <row r="47" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="34">
-        <v>2</v>
-      </c>
-      <c r="B47" s="35" t="s">
-        <v>293</v>
-      </c>
-      <c r="C47" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="D47" s="35" t="str">
-        <f t="shared" si="10"/>
-        <v>numeric</v>
-      </c>
-      <c r="E47" s="35">
-        <v>0</v>
-      </c>
-      <c r="F47" s="36">
-        <v>700</v>
-      </c>
-      <c r="G47" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="H47" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="I47" s="35"/>
-      <c r="J47" s="35">
-        <v>0</v>
-      </c>
-      <c r="K47" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="L47" s="35">
-        <v>24</v>
-      </c>
-      <c r="M47" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="N47" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="O47" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="P47" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q47" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="R47" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="S47" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="T47" s="38"/>
-    </row>
-    <row r="48" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="34">
-        <v>30</v>
-      </c>
-      <c r="B48" s="34" t="s">
-        <v>69</v>
+      <c r="B48" s="35" t="s">
+        <v>291</v>
       </c>
       <c r="C48" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D48" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D48:D49" si="11">LEFT(C48, FIND("-", C48)-1)</f>
         <v>numeric</v>
       </c>
       <c r="E48" s="35">
         <v>0</v>
       </c>
-      <c r="F48" s="34">
-        <v>20</v>
-      </c>
-      <c r="G48" s="35" t="s">
+      <c r="F48" s="36">
+        <v>800</v>
+      </c>
+      <c r="G48" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="H48" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="I48" s="34"/>
+      <c r="H48" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="I48" s="35"/>
       <c r="J48" s="34">
         <v>0</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>44</v>
       </c>
       <c r="L48" s="34">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="M48" s="34" t="s">
         <v>44</v>
@@ -4175,41 +4175,41 @@
       </c>
       <c r="T48" s="38"/>
     </row>
-    <row r="49" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="34">
-        <v>31</v>
-      </c>
-      <c r="B49" s="34" t="s">
-        <v>70</v>
+        <v>2</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>292</v>
       </c>
       <c r="C49" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="35" t="str">
-        <f t="shared" ref="D49:D80" si="11">LEFT(C49, FIND("-", C49)-1)</f>
+        <f t="shared" si="11"/>
         <v>numeric</v>
       </c>
       <c r="E49" s="35">
         <v>0</v>
       </c>
-      <c r="F49" s="34">
-        <v>6</v>
-      </c>
-      <c r="G49" s="35" t="s">
+      <c r="F49" s="36">
+        <v>700</v>
+      </c>
+      <c r="G49" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="H49" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="I49" s="34"/>
-      <c r="J49" s="34">
+      <c r="H49" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35">
         <v>0</v>
       </c>
       <c r="K49" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="L49" s="34">
-        <v>72</v>
+      <c r="L49" s="35">
+        <v>24</v>
       </c>
       <c r="M49" s="34" t="s">
         <v>44</v>
@@ -4236,16 +4236,16 @@
     </row>
     <row r="50" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="34">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C50" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D50" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="0"/>
         <v>numeric</v>
       </c>
       <c r="E50" s="35">
@@ -4295,23 +4295,23 @@
     </row>
     <row r="51" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="34">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B51" s="34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C51" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D51" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="D51:D82" si="12">LEFT(C51, FIND("-", C51)-1)</f>
         <v>numeric</v>
       </c>
       <c r="E51" s="35">
         <v>0</v>
       </c>
       <c r="F51" s="34">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="G51" s="35" t="s">
         <v>10</v>
@@ -4354,23 +4354,23 @@
     </row>
     <row r="52" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="34">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B52" s="34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C52" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D52" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E52" s="35">
         <v>0</v>
       </c>
       <c r="F52" s="34">
-        <v>140</v>
+        <v>20</v>
       </c>
       <c r="G52" s="35" t="s">
         <v>10</v>
@@ -4413,23 +4413,23 @@
     </row>
     <row r="53" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="34">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B53" s="34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C53" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D53" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E53" s="35">
         <v>0</v>
       </c>
       <c r="F53" s="34">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="G53" s="35" t="s">
         <v>10</v>
@@ -4470,27 +4470,27 @@
       </c>
       <c r="T53" s="38"/>
     </row>
-    <row r="54" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="34">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B54" s="34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C54" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D54" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E54" s="35">
         <v>0</v>
       </c>
       <c r="F54" s="34">
-        <v>10</v>
-      </c>
-      <c r="G54" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="G54" s="35" t="s">
         <v>10</v>
       </c>
       <c r="H54" s="34" t="s">
@@ -4529,27 +4529,27 @@
       </c>
       <c r="T54" s="38"/>
     </row>
-    <row r="55" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="34">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B55" s="34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C55" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D55" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E55" s="35">
         <v>0</v>
       </c>
       <c r="F55" s="34">
-        <v>100</v>
-      </c>
-      <c r="G55" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="G55" s="35" t="s">
         <v>10</v>
       </c>
       <c r="H55" s="34" t="s">
@@ -4590,23 +4590,23 @@
     </row>
     <row r="56" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="34">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B56" s="34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C56" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D56" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E56" s="35">
         <v>0</v>
       </c>
       <c r="F56" s="34">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G56" s="36" t="s">
         <v>10</v>
@@ -4649,23 +4649,23 @@
     </row>
     <row r="57" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="34">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B57" s="34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C57" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D57" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E57" s="35">
         <v>0</v>
       </c>
       <c r="F57" s="34">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="G57" s="36" t="s">
         <v>10</v>
@@ -4708,23 +4708,23 @@
     </row>
     <row r="58" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="34">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C58" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D58" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E58" s="35">
         <v>0</v>
       </c>
       <c r="F58" s="34">
-        <v>1100</v>
+        <v>15</v>
       </c>
       <c r="G58" s="36" t="s">
         <v>10</v>
@@ -4767,23 +4767,23 @@
     </row>
     <row r="59" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="34">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B59" s="34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C59" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D59" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E59" s="35">
         <v>0</v>
       </c>
       <c r="F59" s="34">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G59" s="36" t="s">
         <v>10</v>
@@ -4826,23 +4826,23 @@
     </row>
     <row r="60" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="34">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B60" s="34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C60" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D60" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E60" s="35">
         <v>0</v>
       </c>
       <c r="F60" s="34">
-        <v>20</v>
+        <v>1100</v>
       </c>
       <c r="G60" s="36" t="s">
         <v>10</v>
@@ -4885,23 +4885,23 @@
     </row>
     <row r="61" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="34">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B61" s="34" t="s">
-        <v>291</v>
+        <v>80</v>
       </c>
       <c r="C61" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D61" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E61" s="35">
         <v>0</v>
       </c>
       <c r="F61" s="34">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G61" s="36" t="s">
         <v>10</v>
@@ -4944,23 +4944,23 @@
     </row>
     <row r="62" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="34">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B62" s="34" t="s">
-        <v>290</v>
+        <v>81</v>
       </c>
       <c r="C62" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D62" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E62" s="35">
         <v>0</v>
       </c>
       <c r="F62" s="34">
-        <v>40000</v>
+        <v>20</v>
       </c>
       <c r="G62" s="36" t="s">
         <v>10</v>
@@ -5003,23 +5003,23 @@
     </row>
     <row r="63" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="34">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B63" s="34" t="s">
-        <v>82</v>
+        <v>290</v>
       </c>
       <c r="C63" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D63" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E63" s="35">
         <v>0</v>
       </c>
       <c r="F63" s="34">
-        <v>350</v>
+        <v>15</v>
       </c>
       <c r="G63" s="36" t="s">
         <v>10</v>
@@ -5062,7 +5062,7 @@
     </row>
     <row r="64" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="34">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B64" s="34" t="s">
         <v>289</v>
@@ -5071,14 +5071,14 @@
         <v>28</v>
       </c>
       <c r="D64" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E64" s="35">
         <v>0</v>
       </c>
       <c r="F64" s="34">
-        <v>100</v>
+        <v>40000</v>
       </c>
       <c r="G64" s="36" t="s">
         <v>10</v>
@@ -5121,23 +5121,23 @@
     </row>
     <row r="65" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="34">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B65" s="34" t="s">
-        <v>288</v>
+        <v>82</v>
       </c>
       <c r="C65" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D65" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E65" s="35">
         <v>0</v>
       </c>
       <c r="F65" s="34">
-        <v>5000</v>
+        <v>350</v>
       </c>
       <c r="G65" s="36" t="s">
         <v>10</v>
@@ -5180,23 +5180,23 @@
     </row>
     <row r="66" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="34">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B66" s="34" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C66" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D66" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E66" s="35">
         <v>0</v>
       </c>
       <c r="F66" s="34">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="G66" s="36" t="s">
         <v>10</v>
@@ -5239,23 +5239,23 @@
     </row>
     <row r="67" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="34">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B67" s="34" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C67" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D67" s="35" t="str">
-        <f t="shared" ref="D67" si="12">LEFT(C67, FIND("-", C67)-1)</f>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E67" s="35">
         <v>0</v>
       </c>
       <c r="F67" s="34">
-        <v>250</v>
+        <v>5000</v>
       </c>
       <c r="G67" s="36" t="s">
         <v>10</v>
@@ -5298,23 +5298,23 @@
     </row>
     <row r="68" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="34">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B68" s="34" t="s">
-        <v>83</v>
+        <v>286</v>
       </c>
       <c r="C68" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D68" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E68" s="35">
         <v>0</v>
       </c>
       <c r="F68" s="34">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="G68" s="36" t="s">
         <v>10</v>
@@ -5357,23 +5357,23 @@
     </row>
     <row r="69" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="34">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B69" s="34" t="s">
-        <v>84</v>
+        <v>285</v>
       </c>
       <c r="C69" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D69" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="D69" si="13">LEFT(C69, FIND("-", C69)-1)</f>
         <v>numeric</v>
       </c>
       <c r="E69" s="35">
         <v>0</v>
       </c>
       <c r="F69" s="34">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="G69" s="36" t="s">
         <v>10</v>
@@ -5416,23 +5416,23 @@
     </row>
     <row r="70" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="34">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B70" s="34" t="s">
-        <v>284</v>
+        <v>83</v>
       </c>
       <c r="C70" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D70" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E70" s="35">
         <v>0</v>
       </c>
       <c r="F70" s="34">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="G70" s="36" t="s">
         <v>10</v>
@@ -5448,7 +5448,7 @@
         <v>44</v>
       </c>
       <c r="L70" s="34">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="M70" s="34" t="s">
         <v>44</v>
@@ -5475,16 +5475,16 @@
     </row>
     <row r="71" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="34">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B71" s="34" t="s">
-        <v>285</v>
+        <v>84</v>
       </c>
       <c r="C71" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D71" s="35" t="str">
-        <f t="shared" ref="D71" si="13">LEFT(C71, FIND("-", C71)-1)</f>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E71" s="35">
@@ -5507,7 +5507,7 @@
         <v>44</v>
       </c>
       <c r="L71" s="34">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="M71" s="34" t="s">
         <v>44</v>
@@ -5534,23 +5534,23 @@
     </row>
     <row r="72" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="34">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B72" s="34" t="s">
-        <v>85</v>
+        <v>283</v>
       </c>
       <c r="C72" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D72" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E72" s="35">
         <v>0</v>
       </c>
       <c r="F72" s="34">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="G72" s="36" t="s">
         <v>10</v>
@@ -5566,7 +5566,7 @@
         <v>44</v>
       </c>
       <c r="L72" s="34">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="M72" s="34" t="s">
         <v>44</v>
@@ -5593,23 +5593,23 @@
     </row>
     <row r="73" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="34">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B73" s="34" t="s">
-        <v>86</v>
+        <v>284</v>
       </c>
       <c r="C73" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D73" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="D73" si="14">LEFT(C73, FIND("-", C73)-1)</f>
         <v>numeric</v>
       </c>
       <c r="E73" s="35">
         <v>0</v>
       </c>
       <c r="F73" s="34">
-        <v>60</v>
+        <v>1000</v>
       </c>
       <c r="G73" s="36" t="s">
         <v>10</v>
@@ -5625,7 +5625,7 @@
         <v>44</v>
       </c>
       <c r="L73" s="34">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="M73" s="34" t="s">
         <v>44</v>
@@ -5652,23 +5652,23 @@
     </row>
     <row r="74" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="34">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B74" s="34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C74" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D74" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E74" s="35">
         <v>0</v>
       </c>
       <c r="F74" s="34">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="G74" s="36" t="s">
         <v>10</v>
@@ -5711,23 +5711,23 @@
     </row>
     <row r="75" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="34">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B75" s="34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C75" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D75" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E75" s="35">
         <v>0</v>
       </c>
       <c r="F75" s="34">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="G75" s="36" t="s">
         <v>10</v>
@@ -5743,7 +5743,7 @@
         <v>44</v>
       </c>
       <c r="L75" s="34">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="M75" s="34" t="s">
         <v>44</v>
@@ -5770,23 +5770,23 @@
     </row>
     <row r="76" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="34">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B76" s="34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C76" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D76" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E76" s="35">
         <v>0</v>
       </c>
       <c r="F76" s="34">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="G76" s="36" t="s">
         <v>10</v>
@@ -5802,7 +5802,7 @@
         <v>44</v>
       </c>
       <c r="L76" s="34">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="M76" s="34" t="s">
         <v>44</v>
@@ -5829,23 +5829,23 @@
     </row>
     <row r="77" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="34">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B77" s="34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C77" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D77" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E77" s="35">
         <v>0</v>
       </c>
       <c r="F77" s="34">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="G77" s="36" t="s">
         <v>10</v>
@@ -5888,16 +5888,16 @@
     </row>
     <row r="78" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="34">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B78" s="34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C78" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D78" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E78" s="35">
@@ -5920,7 +5920,7 @@
         <v>44</v>
       </c>
       <c r="L78" s="34">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="M78" s="34" t="s">
         <v>44</v>
@@ -5947,23 +5947,23 @@
     </row>
     <row r="79" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="34">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B79" s="34" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C79" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D79" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E79" s="35">
         <v>0</v>
       </c>
       <c r="F79" s="34">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="G79" s="36" t="s">
         <v>10</v>
@@ -5979,7 +5979,7 @@
         <v>44</v>
       </c>
       <c r="L79" s="34">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="M79" s="34" t="s">
         <v>44</v>
@@ -6006,23 +6006,23 @@
     </row>
     <row r="80" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="34">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B80" s="34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C80" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D80" s="35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E80" s="35">
         <v>0</v>
       </c>
       <c r="F80" s="34">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="G80" s="36" t="s">
         <v>10</v>
@@ -6038,10 +6038,10 @@
         <v>44</v>
       </c>
       <c r="L80" s="34">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="M80" s="34" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="N80" s="37" t="s">
         <v>45</v>
@@ -6065,23 +6065,23 @@
     </row>
     <row r="81" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="34">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B81" s="34" t="s">
-        <v>168</v>
+        <v>92</v>
       </c>
       <c r="C81" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D81" s="35" t="str">
-        <f t="shared" ref="D81:D82" si="14">LEFT(C81, FIND("-", C81)-1)</f>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E81" s="35">
         <v>0</v>
       </c>
       <c r="F81" s="34">
-        <v>50000</v>
+        <v>200</v>
       </c>
       <c r="G81" s="36" t="s">
         <v>10</v>
@@ -6124,23 +6124,23 @@
     </row>
     <row r="82" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="34">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B82" s="34" t="s">
-        <v>169</v>
+        <v>93</v>
       </c>
       <c r="C82" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D82" s="35" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>numeric</v>
       </c>
       <c r="E82" s="35">
         <v>0</v>
       </c>
       <c r="F82" s="34">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="G82" s="36" t="s">
         <v>10</v>
@@ -6156,10 +6156,10 @@
         <v>44</v>
       </c>
       <c r="L82" s="34">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="M82" s="34" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="N82" s="37" t="s">
         <v>45</v>
@@ -6183,10 +6183,10 @@
     </row>
     <row r="83" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="34">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B83" s="34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C83" s="35" t="s">
         <v>28</v>
@@ -6199,7 +6199,7 @@
         <v>0</v>
       </c>
       <c r="F83" s="34">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="G83" s="36" t="s">
         <v>10</v>
@@ -6242,10 +6242,10 @@
     </row>
     <row r="84" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="34">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B84" s="34" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C84" s="35" t="s">
         <v>28</v>
@@ -6258,7 +6258,7 @@
         <v>0</v>
       </c>
       <c r="F84" s="34">
-        <v>10000</v>
+        <v>600</v>
       </c>
       <c r="G84" s="36" t="s">
         <v>10</v>
@@ -6274,7 +6274,7 @@
         <v>44</v>
       </c>
       <c r="L84" s="34">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="M84" s="34" t="s">
         <v>44</v>
@@ -6301,10 +6301,10 @@
     </row>
     <row r="85" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="34">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B85" s="34" t="s">
-        <v>278</v>
+        <v>170</v>
       </c>
       <c r="C85" s="35" t="s">
         <v>28</v>
@@ -6317,7 +6317,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="34">
-        <v>150</v>
+        <v>10000</v>
       </c>
       <c r="G85" s="36" t="s">
         <v>10</v>
@@ -6360,10 +6360,10 @@
     </row>
     <row r="86" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="34">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B86" s="34" t="s">
-        <v>279</v>
+        <v>171</v>
       </c>
       <c r="C86" s="35" t="s">
         <v>28</v>
@@ -6376,7 +6376,7 @@
         <v>0</v>
       </c>
       <c r="F86" s="34">
-        <v>150</v>
+        <v>10000</v>
       </c>
       <c r="G86" s="36" t="s">
         <v>10</v>
@@ -6418,48 +6418,122 @@
       <c r="T86" s="38"/>
     </row>
     <row r="87" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3"/>
-      <c r="I87" s="3"/>
-      <c r="J87" s="3"/>
-      <c r="K87" s="3"/>
-      <c r="L87" s="3"/>
-      <c r="M87" s="3"/>
-      <c r="N87" s="14"/>
-      <c r="O87" s="14"/>
-      <c r="P87" s="14"/>
-      <c r="Q87" s="14"/>
-      <c r="R87" s="14"/>
-      <c r="S87" s="14"/>
-      <c r="T87" s="4"/>
+      <c r="A87" s="34">
+        <v>68</v>
+      </c>
+      <c r="B87" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="C87" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D87" s="35" t="str">
+        <f t="shared" ref="D87:D88" si="17">LEFT(C87, FIND("-", C87)-1)</f>
+        <v>numeric</v>
+      </c>
+      <c r="E87" s="35">
+        <v>0</v>
+      </c>
+      <c r="F87" s="34">
+        <v>150</v>
+      </c>
+      <c r="G87" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="H87" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I87" s="34"/>
+      <c r="J87" s="34">
+        <v>0</v>
+      </c>
+      <c r="K87" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="L87" s="34">
+        <v>72</v>
+      </c>
+      <c r="M87" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="N87" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="O87" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="P87" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q87" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="R87" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="S87" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="T87" s="38"/>
     </row>
     <row r="88" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
-      <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
-      <c r="J88" s="3"/>
-      <c r="K88" s="3"/>
-      <c r="L88" s="3"/>
-      <c r="M88" s="3"/>
-      <c r="N88" s="14"/>
-      <c r="O88" s="14"/>
-      <c r="P88" s="14"/>
-      <c r="Q88" s="14"/>
-      <c r="R88" s="14"/>
-      <c r="S88" s="14"/>
-      <c r="T88" s="4"/>
+      <c r="A88" s="34">
+        <v>69</v>
+      </c>
+      <c r="B88" s="34" t="s">
+        <v>278</v>
+      </c>
+      <c r="C88" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D88" s="35" t="str">
+        <f t="shared" si="17"/>
+        <v>numeric</v>
+      </c>
+      <c r="E88" s="35">
+        <v>0</v>
+      </c>
+      <c r="F88" s="34">
+        <v>150</v>
+      </c>
+      <c r="G88" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="H88" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I88" s="34"/>
+      <c r="J88" s="34">
+        <v>0</v>
+      </c>
+      <c r="K88" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="L88" s="34">
+        <v>72</v>
+      </c>
+      <c r="M88" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="N88" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="O88" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="P88" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q88" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="R88" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="S88" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="T88" s="38"/>
     </row>
     <row r="89" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
@@ -9231,7 +9305,7 @@
       <c r="Q214" s="14"/>
       <c r="R214" s="14"/>
       <c r="S214" s="14"/>
-      <c r="T214" s="3"/>
+      <c r="T214" s="4"/>
     </row>
     <row r="215" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3"/>
@@ -9253,7 +9327,7 @@
       <c r="Q215" s="14"/>
       <c r="R215" s="14"/>
       <c r="S215" s="14"/>
-      <c r="T215" s="3"/>
+      <c r="T215" s="4"/>
     </row>
     <row r="216" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3"/>
@@ -24479,8 +24553,52 @@
       <c r="S907" s="14"/>
       <c r="T907" s="3"/>
     </row>
+    <row r="908" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A908" s="3"/>
+      <c r="B908" s="3"/>
+      <c r="C908" s="3"/>
+      <c r="D908" s="3"/>
+      <c r="E908" s="3"/>
+      <c r="F908" s="3"/>
+      <c r="G908" s="3"/>
+      <c r="H908" s="3"/>
+      <c r="I908" s="3"/>
+      <c r="J908" s="3"/>
+      <c r="K908" s="3"/>
+      <c r="L908" s="3"/>
+      <c r="M908" s="3"/>
+      <c r="N908" s="14"/>
+      <c r="O908" s="14"/>
+      <c r="P908" s="14"/>
+      <c r="Q908" s="14"/>
+      <c r="R908" s="14"/>
+      <c r="S908" s="14"/>
+      <c r="T908" s="3"/>
+    </row>
+    <row r="909" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A909" s="3"/>
+      <c r="B909" s="3"/>
+      <c r="C909" s="3"/>
+      <c r="D909" s="3"/>
+      <c r="E909" s="3"/>
+      <c r="F909" s="3"/>
+      <c r="G909" s="3"/>
+      <c r="H909" s="3"/>
+      <c r="I909" s="3"/>
+      <c r="J909" s="3"/>
+      <c r="K909" s="3"/>
+      <c r="L909" s="3"/>
+      <c r="M909" s="3"/>
+      <c r="N909" s="14"/>
+      <c r="O909" s="14"/>
+      <c r="P909" s="14"/>
+      <c r="Q909" s="14"/>
+      <c r="R909" s="14"/>
+      <c r="S909" s="14"/>
+      <c r="T909" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:T907" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:T909" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataValidations count="5">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{0BA62E2C-90D0-4A85-8B8A-6B7F0EEA38EF}">
       <formula1>0</formula1>
@@ -24508,11 +24626,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X1018"/>
+  <dimension ref="A1:X1017"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24583,7 +24701,7 @@
         <v>1104</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>23</v>
@@ -24616,7 +24734,7 @@
         <v>1105</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -24649,13 +24767,13 @@
         <v>1101</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>225</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>226</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>45</v>
@@ -24683,7 +24801,7 @@
         <v>1170</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C5" s="3">
         <v>70</v>
@@ -24713,11 +24831,11 @@
     </row>
     <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <f t="shared" ref="A6:A36" si="0">1100+C6</f>
+        <f t="shared" ref="A6:A35" si="0">1100+C6</f>
         <v>1172</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C6" s="3">
         <v>72</v>
@@ -24751,7 +24869,7 @@
         <v>1173</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C7" s="3">
         <v>73</v>
@@ -24785,7 +24903,7 @@
         <v>1174</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C8" s="3">
         <v>74</v>
@@ -24819,7 +24937,7 @@
         <v>1175</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C9" s="3">
         <v>75</v>
@@ -24853,7 +24971,7 @@
         <v>1176</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C10" s="3">
         <v>76</v>
@@ -24887,7 +25005,7 @@
         <v>1177</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C11" s="3">
         <v>77</v>
@@ -24921,7 +25039,7 @@
         <v>1178</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C12" s="3">
         <v>78</v>
@@ -24955,7 +25073,7 @@
         <v>1179</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C13" s="3">
         <v>79</v>
@@ -24989,7 +25107,7 @@
         <v>1180</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C14" s="3">
         <v>80</v>
@@ -25564,13 +25682,13 @@
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>192</v>
       </c>
       <c r="C31" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>102</v>
@@ -25598,13 +25716,13 @@
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <f t="shared" si="0"/>
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>193</v>
       </c>
       <c r="C32" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>102</v>
@@ -25632,13 +25750,13 @@
     <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <f t="shared" si="0"/>
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
       <c r="C33" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>102</v>
@@ -25666,13 +25784,13 @@
     <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <f t="shared" si="0"/>
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="C34" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>102</v>
@@ -25700,13 +25818,13 @@
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <f t="shared" si="0"/>
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>195</v>
       </c>
       <c r="C35" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>102</v>
@@ -25733,14 +25851,13 @@
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <f t="shared" si="0"/>
-        <v>1124</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>196</v>
+        <v>1188</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>349</v>
       </c>
       <c r="C36" s="3">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>102</v>
@@ -25766,16 +25883,36 @@
       <c r="K36" s="3"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
+      <c r="A37" s="3">
+        <v>1189</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C37" s="3">
+        <v>89</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="K37" s="3"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -38518,25 +38655,12 @@
       <c r="J1017" s="14"/>
       <c r="K1017" s="3"/>
     </row>
-    <row r="1018" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1018" s="3"/>
-      <c r="B1018" s="3"/>
-      <c r="C1018" s="3"/>
-      <c r="D1018" s="3"/>
-      <c r="E1018" s="14"/>
-      <c r="F1018" s="14"/>
-      <c r="G1018" s="14"/>
-      <c r="H1018" s="14"/>
-      <c r="I1018" s="14"/>
-      <c r="J1018" s="14"/>
-      <c r="K1018" s="3"/>
-    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576 C15:C36" xr:uid="{98A4E0C0-623A-43B0-A1B2-0ACD9C28F3FC}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Error" error="Currently, The implementation requires a derived from concept id, but the program is not planned to deal with TAKs that have more then 1 base concepts. Please focus on one at the time, or contact developers." sqref="C5:C14" xr:uid="{60DADC71-9D75-41E9-8E91-4A0A84ACE9E1}"/>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C35 A2:A1048576" xr:uid="{98A4E0C0-623A-43B0-A1B2-0ACD9C28F3FC}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Error" error="Currently, The implementation requires a derived from concept id, but the program is not planned to deal with TAKs that have more then 1 base concepts. Please focus on one at the time, or contact developers." sqref="C5:C14" xr:uid="{60DADC71-9D75-41E9-8E91-4A0A84ACE9E1}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:J1048576" xr:uid="{BD14D827-2ED4-418B-B045-D2154EB50A63}">
       <formula1>"true, false"</formula1>
     </dataValidation>
@@ -38555,7 +38679,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -38663,7 +38787,7 @@
         <v>1203</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2" s="19">
         <v>3</v>
@@ -38715,7 +38839,7 @@
         <v>1225</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" s="3">
         <v>25</v>
@@ -38759,7 +38883,7 @@
         <v>1226</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4" s="23">
         <v>26</v>
@@ -38803,7 +38927,7 @@
         <v>1227</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C5" s="23">
         <v>27</v>
@@ -38847,7 +38971,7 @@
         <v>1228</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6" s="23">
         <v>28</v>
@@ -38886,7 +39010,50 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23">
+        <v>1219</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C7" s="23">
+        <v>19</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="19">
+        <v>0</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="R7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="S7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="T7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="U7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="V7" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -39891,17 +40058,17 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{F7A19A48-EA19-43B2-96D8-8F3C8A8E029D}">
       <formula1>"equal, not-equal, bigger-equal, bigger, smaller-equal, smaller"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576 I2:I1048576 N2:N1048576" xr:uid="{1C156D25-1B38-4894-84AB-46AD25227753}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576 I2:I1048576 F2:F1048576" xr:uid="{1C156D25-1B38-4894-84AB-46AD25227753}">
       <formula1>"start, end"</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{E865A148-F093-421F-AB63-585CEEC96279}">
       <formula1>-1000000000000</formula1>
       <formula2>1000000000000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576 K2:K1048576 P2:P1048576" xr:uid="{67414E21-2133-4E5E-B5D4-E1052B042939}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P1048576 K2:K1048576 H2:H1048576" xr:uid="{67414E21-2133-4E5E-B5D4-E1052B042939}">
       <formula1>"second, minute, hour, day, week, month, year"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576 J2:J1048576" xr:uid="{E5AEA31F-71B0-477A-8372-81A09F350705}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576 O2:O1048576" xr:uid="{E5AEA31F-71B0-477A-8372-81A09F350705}">
       <formula1>-100000000000</formula1>
       <formula2>100000000000</formula2>
     </dataValidation>
@@ -40016,7 +40183,7 @@
         <v>1001</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -40072,7 +40239,7 @@
         <v>1002</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
@@ -40084,7 +40251,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>20</v>
@@ -40128,7 +40295,7 @@
         <v>1004</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C4" s="3">
         <v>4</v>
@@ -40140,7 +40307,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>173</v>
@@ -40184,7 +40351,7 @@
         <v>1005</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C5" s="3">
         <v>5</v>
@@ -40196,7 +40363,7 @@
         <v>15</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>173</v>
@@ -40240,7 +40407,7 @@
         <v>1063</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C6" s="3">
         <v>63</v>
@@ -40296,7 +40463,7 @@
         <v>1030</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C7" s="3">
         <v>30</v>
@@ -40308,7 +40475,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>119</v>
@@ -40352,7 +40519,7 @@
         <v>1031</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C8" s="3">
         <v>31</v>
@@ -40408,7 +40575,7 @@
         <v>1032</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C9" s="3">
         <v>32</v>
@@ -40420,7 +40587,7 @@
         <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>121</v>
@@ -40464,7 +40631,7 @@
         <v>1033</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C10" s="3">
         <v>33</v>
@@ -40476,7 +40643,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>122</v>
@@ -40520,7 +40687,7 @@
         <v>1034</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C11" s="3">
         <v>34</v>
@@ -40532,10 +40699,10 @@
         <v>15</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H11" s="3">
         <v>0</v>
@@ -40576,7 +40743,7 @@
         <v>1035</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C12" s="3">
         <v>35</v>
@@ -40588,7 +40755,7 @@
         <v>15</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>122</v>
@@ -40632,7 +40799,7 @@
         <v>1036</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C13" s="3">
         <v>36</v>
@@ -40644,10 +40811,10 @@
         <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>265</v>
       </c>
       <c r="H13" s="3">
         <v>0</v>
@@ -40688,7 +40855,7 @@
         <v>1037</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C14" s="3">
         <v>37</v>
@@ -40744,7 +40911,7 @@
         <v>1038</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C15" s="3">
         <v>38</v>
@@ -40756,7 +40923,7 @@
         <v>15</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>125</v>
@@ -40800,7 +40967,7 @@
         <v>1039</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C16" s="3">
         <v>39</v>
@@ -40812,7 +40979,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>122</v>
@@ -40856,7 +41023,7 @@
         <v>1040</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C17" s="3">
         <v>40</v>
@@ -40868,7 +41035,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>126</v>
@@ -40912,7 +41079,7 @@
         <v>1041</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C18" s="3">
         <v>41</v>
@@ -40924,7 +41091,7 @@
         <v>15</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>127</v>
@@ -40968,7 +41135,7 @@
         <v>1042</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C19" s="3">
         <v>42</v>
@@ -40980,7 +41147,7 @@
         <v>15</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>128</v>
@@ -41024,7 +41191,7 @@
         <v>1043</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C20" s="3">
         <v>43</v>
@@ -41036,7 +41203,7 @@
         <v>15</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>129</v>
@@ -41080,7 +41247,7 @@
         <v>1044</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C21" s="3">
         <v>44</v>
@@ -41092,7 +41259,7 @@
         <v>15</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>130</v>
@@ -41136,7 +41303,7 @@
         <v>1045</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C22" s="3">
         <v>45</v>
@@ -41148,7 +41315,7 @@
         <v>15</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>122</v>
@@ -41192,7 +41359,7 @@
         <v>1046</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C23" s="3">
         <v>46</v>
@@ -41204,7 +41371,7 @@
         <v>15</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>131</v>
@@ -41248,7 +41415,7 @@
         <v>1047</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C24" s="3">
         <v>47</v>
@@ -41260,7 +41427,7 @@
         <v>15</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>132</v>
@@ -41304,7 +41471,7 @@
         <v>1048</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C25" s="3">
         <v>48</v>
@@ -41360,7 +41527,7 @@
         <v>1049</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C26" s="3">
         <v>49</v>
@@ -41372,10 +41539,10 @@
         <v>15</v>
       </c>
       <c r="F26" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>273</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="H26" s="3">
         <v>0</v>
@@ -41416,7 +41583,7 @@
         <v>1050</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C27" s="3">
         <v>50</v>
@@ -41472,7 +41639,7 @@
         <v>1051</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C28" s="3">
         <v>51</v>
@@ -41528,7 +41695,7 @@
         <v>1052</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C29" s="3">
         <v>52</v>
@@ -41584,7 +41751,7 @@
         <v>1053</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C30" s="3">
         <v>53</v>
@@ -41640,7 +41807,7 @@
         <v>1054</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C31" s="3">
         <v>54</v>
@@ -41696,7 +41863,7 @@
         <v>1055</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C32" s="3">
         <v>55</v>
@@ -41708,7 +41875,7 @@
         <v>15</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>143</v>
@@ -41752,7 +41919,7 @@
         <v>1057</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C33" s="3">
         <v>57</v>
@@ -41808,7 +41975,7 @@
         <v>1058</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C34" s="3">
         <v>58</v>
@@ -41820,7 +41987,7 @@
         <v>15</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>145</v>
@@ -41864,7 +42031,7 @@
         <v>1059</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C35" s="3">
         <v>59</v>
@@ -41876,7 +42043,7 @@
         <v>15</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>145</v>
@@ -41920,7 +42087,7 @@
         <v>1060</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C36" s="3">
         <v>60</v>
@@ -41932,7 +42099,7 @@
         <v>15</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>145</v>
@@ -41976,7 +42143,7 @@
         <v>1061</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C37" s="3">
         <v>61</v>
@@ -42032,7 +42199,7 @@
         <v>1062</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C38" s="3">
         <v>62</v>
@@ -42088,7 +42255,7 @@
         <v>1064</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C39" s="3">
         <v>64</v>
@@ -42100,7 +42267,7 @@
         <v>15</v>
       </c>
       <c r="F39" s="39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>175</v>
@@ -42144,7 +42311,7 @@
         <v>1065</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C40" s="3">
         <v>65</v>
@@ -42156,10 +42323,10 @@
         <v>15</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H40" s="3">
         <v>0</v>
@@ -42200,7 +42367,7 @@
         <v>1066</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C41" s="3">
         <v>66</v>
@@ -42212,10 +42379,10 @@
         <v>15</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H41" s="3">
         <v>0</v>
@@ -42256,7 +42423,7 @@
         <v>1067</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C42" s="3">
         <v>67</v>
@@ -42268,10 +42435,10 @@
         <v>15</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H42" s="3">
         <v>0</v>
@@ -42312,7 +42479,7 @@
         <v>1068</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C43" s="3">
         <v>68</v>
@@ -42324,10 +42491,10 @@
         <v>15</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H43" s="3">
         <v>0</v>
@@ -42368,7 +42535,7 @@
         <v>1069</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C44" s="3">
         <v>69</v>
@@ -42380,10 +42547,10 @@
         <v>15</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H44" s="3">
         <v>0</v>
@@ -42424,7 +42591,7 @@
         <v>1071</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C45" s="3">
         <v>71</v>
@@ -42478,7 +42645,7 @@
         <v>1081</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C46" s="3">
         <v>81</v>
@@ -42532,7 +42699,7 @@
         <v>1082</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C47" s="3">
         <v>82</v>
@@ -60620,7 +60787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A161545-DA5F-4FD2-8279-D89A8EE73974}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -60645,13 +60812,13 @@
         <v>13</v>
       </c>
       <c r="D1" s="40" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="40" t="s">
         <v>222</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="F1" s="40" t="s">
         <v>223</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -60660,7 +60827,7 @@
         <v>2401</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C2" s="3">
         <v>1101</v>
@@ -60681,7 +60848,7 @@
         <v>1301</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -60703,7 +60870,7 @@
         <v>1302</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C4" s="3">
         <v>2</v>
@@ -60725,7 +60892,7 @@
         <v>1330</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C5" s="3">
         <v>30</v>
@@ -60747,7 +60914,7 @@
         <v>1333</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C6" s="3">
         <v>33</v>
@@ -60769,7 +60936,7 @@
         <v>1336</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C7" s="3">
         <v>36</v>
@@ -60791,7 +60958,7 @@
         <v>1337</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C8" s="3">
         <v>37</v>
@@ -60813,7 +60980,7 @@
         <v>1338</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C9" s="3">
         <v>38</v>
@@ -60835,7 +61002,7 @@
         <v>1340</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C10" s="3">
         <v>40</v>
@@ -60857,7 +61024,7 @@
         <v>1343</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C11" s="3">
         <v>43</v>
@@ -60879,7 +61046,7 @@
         <v>1344</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C12" s="3">
         <v>44</v>
@@ -60901,7 +61068,7 @@
         <v>1345</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C13" s="3">
         <v>45</v>
@@ -60924,7 +61091,7 @@
         <v>1346</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C14" s="3">
         <v>46</v>
@@ -60947,7 +61114,7 @@
         <v>1347</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C15" s="3">
         <v>47</v>
@@ -60970,7 +61137,7 @@
         <v>1348</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C16" s="3">
         <v>48</v>
@@ -60992,7 +61159,7 @@
         <v>1350</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C17" s="3">
         <v>50</v>
@@ -61014,7 +61181,7 @@
         <v>1351</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C18" s="3">
         <v>51</v>
@@ -61036,7 +61203,7 @@
         <v>1352</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C19" s="3">
         <v>52</v>
@@ -61058,7 +61225,7 @@
         <v>1353</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C20" s="3">
         <v>53</v>
@@ -61080,7 +61247,7 @@
         <v>1354</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C21" s="3">
         <v>54</v>
@@ -61102,7 +61269,7 @@
         <v>1355</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C22" s="3">
         <v>55</v>
@@ -61124,7 +61291,7 @@
         <v>1357</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C23" s="3">
         <v>57</v>
@@ -61146,7 +61313,7 @@
         <v>1358</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C24" s="3">
         <v>58</v>
@@ -61168,7 +61335,7 @@
         <v>1359</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C25" s="3">
         <v>59</v>
@@ -61190,7 +61357,7 @@
         <v>1360</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C26" s="3">
         <v>60</v>
@@ -61212,7 +61379,7 @@
         <v>1361</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C27" s="3">
         <v>61</v>
@@ -61234,7 +61401,7 @@
         <v>1362</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C28" s="3">
         <v>62</v>
@@ -61257,7 +61424,7 @@
         <v>1364</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C29" s="3">
         <v>64</v>
@@ -61279,7 +61446,7 @@
         <v>1366</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C30" s="3">
         <v>66</v>
@@ -61301,7 +61468,7 @@
         <v>1367</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C31" s="3">
         <v>67</v>

</xml_diff>

<commit_message>
ensure tak_automator ignores no ID rows
</commit_message>
<xml_diff>
--- a/taks.xlsx
+++ b/taks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonat\CodeProjects\TAKAutomator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC004DDD-B68D-46ED-A11F-D4A069960D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C4652B-3D1D-416D-98EB-9C09C6BAD67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_concepts" sheetId="1" r:id="rId1"/>
@@ -24702,8 +24702,8 @@
   </sheetPr>
   <dimension ref="A1:X1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -38403,9 +38403,9 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix validation on trends
</commit_message>
<xml_diff>
--- a/taks.xlsx
+++ b/taks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonat\CodeProjects\TAKAutomator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C4652B-3D1D-416D-98EB-9C09C6BAD67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696819AB-C891-4D76-9495-DECEF369670F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_concepts" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="285">
   <si>
     <t>TYPE</t>
   </si>
@@ -850,12 +850,6 @@
     <t>["Thrombocytopenia", "Normal", "Thrombocytosis"]</t>
   </si>
   <si>
-    <t>LOCAL_PERSISTENCE_GOOD_AFTER_UNIT</t>
-  </si>
-  <si>
-    <t>LOCAL_PERSISTENCE_GOOD_BEFORE_UNIT</t>
-  </si>
-  <si>
     <t>GLUCOSE_MEASURE</t>
   </si>
   <si>
@@ -2386,7 +2380,7 @@
         <v>86</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>24</v>
@@ -2439,7 +2433,7 @@
         <v>87</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>24</v>
@@ -4467,7 +4461,7 @@
         <v>1</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C58" s="34" t="s">
         <v>25</v>
@@ -5796,7 +5790,7 @@
         <v>52</v>
       </c>
       <c r="B81" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C81" s="34" t="s">
         <v>25</v>
@@ -6437,7 +6431,7 @@
         <v>66</v>
       </c>
       <c r="B92" s="33" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C92" s="34" t="s">
         <v>25</v>
@@ -24912,7 +24906,7 @@
         <v>1186</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C6" s="3">
         <v>86</v>
@@ -24946,7 +24940,7 @@
         <v>1187</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C7" s="3">
         <v>87</v>
@@ -38403,7 +38397,7 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
@@ -40215,9 +40209,9 @@
   </sheetPr>
   <dimension ref="A1:AF970"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD4"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -40312,7 +40306,7 @@
         <v>1001</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -40831,7 +40825,7 @@
         <v>1052</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C11" s="3">
         <v>52</v>
@@ -41237,7 +41231,7 @@
         <v>1066</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C18" s="3">
         <v>66</v>
@@ -59635,8 +59629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A161545-DA5F-4FD2-8279-D89A8EE73974}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -59648,7 +59642,7 @@
     <col min="5" max="5" width="24.5546875" customWidth="1"/>
     <col min="6" max="6" width="25.6640625" customWidth="1"/>
     <col min="7" max="7" width="39.88671875" customWidth="1"/>
-    <col min="8" max="8" width="43.77734375" customWidth="1"/>
+    <col min="8" max="8" width="50.33203125" customWidth="1"/>
     <col min="9" max="9" width="42.33203125" customWidth="1"/>
     <col min="10" max="10" width="43.88671875" customWidth="1"/>
   </cols>
@@ -59676,13 +59670,13 @@
         <v>28</v>
       </c>
       <c r="H1" s="39" t="s">
-        <v>274</v>
+        <v>29</v>
       </c>
       <c r="I1" s="39" t="s">
         <v>31</v>
       </c>
       <c r="J1" s="39" t="s">
-        <v>273</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -60032,7 +60026,7 @@
         <v>1352</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C11" s="3">
         <v>52</v>
@@ -60298,7 +60292,7 @@
         <v>1366</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C18" s="3">
         <v>66</v>

</xml_diff>